<commit_message>
updated KNN Classifier notebook
</commit_message>
<xml_diff>
--- a/data/Prediction_Return_Calculator.xlsx
+++ b/data/Prediction_Return_Calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfccdeabb580c92e/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfccdeabb580c92e/AI_Class/GIT/Group_project_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D6F4DE7-2D41-4B1D-ABD0-97ED56768A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{6D6F4DE7-2D41-4B1D-ABD0-97ED56768A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4642A708-6503-4D67-8BBA-4FD5241558F9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{EFDD2668-DBD7-4C0E-92E4-96A70D44951B}"/>
+    <workbookView xWindow="57480" yWindow="3210" windowWidth="38640" windowHeight="21120" xr2:uid="{EFDD2668-DBD7-4C0E-92E4-96A70D44951B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1967,7 +1967,7 @@
   <dimension ref="A1:M501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="I2" sqref="I2:I501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2039,8 +2039,8 @@
         <v>-2.3300000000000125</v>
       </c>
       <c r="I2" s="1">
-        <f>($L$2/COUNT($B$2:$B$501)) * (H2 / B2)</f>
-        <v>-0.35654169854629114</v>
+        <f>($L$2/COUNT($B$2:$B$501)) * (H2 / A2)</f>
+        <v>-0.35029692550552693</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2078,8 +2078,8 @@
         <v>0.18999999999999773</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I66" si="3">($L$2/COUNT($B$2:$B$501)) * (H3 / B3)</f>
-        <v>1.6480895172832348E-2</v>
+        <f t="shared" ref="I3:I66" si="3">($L$2/COUNT($B$2:$B$501)) * (H3 / A3)</f>
+        <v>1.6467325359680859E-2</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="I4" s="1">
         <f t="shared" si="3"/>
-        <v>0.18822661007565936</v>
+        <v>0.19001490312965688</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" si="3"/>
-        <v>-0.12205228659685111</v>
+        <v>-0.12280169799878751</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="3"/>
-        <v>8.0659001201304079E-2</v>
+        <v>8.0335014101358668E-2</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" si="3"/>
-        <v>5.605904886480639E-3</v>
+        <v>5.6074766355142316E-3</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" si="3"/>
-        <v>0.34919153375243711</v>
+        <v>0.34319941720853758</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="M8" s="1">
         <f>SUM(I2:I501)</f>
-        <v>1.6739688009437397</v>
+        <v>3.7999643009219235</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" si="3"/>
-        <v>-9.4458829621956397E-2</v>
+        <v>-9.4014803208047878E-2</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="M9" s="1">
         <f>MAX(I2:I501)</f>
-        <v>3.5994473017578881</v>
+        <v>4.3894219517903128</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" si="3"/>
-        <v>0.24986940623367618</v>
+        <v>0.25303063698479211</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="M10" s="1">
         <f>MIN(I2:I501)</f>
-        <v>-2.470428893905193</v>
+        <v>-2.1988266495218207</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" si="3"/>
-        <v>0.14867256637168202</v>
+        <v>0.14978601997146995</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" si="3"/>
-        <v>3.7305699481866697E-2</v>
+        <v>3.7236243276790815E-2</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" si="3"/>
-        <v>3.2886680894239746E-2</v>
+        <v>3.2832692979394153E-2</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" si="3"/>
-        <v>4.4943820224719738E-2</v>
+        <v>4.4843049327354889E-2</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" si="3"/>
-        <v>-0.28568554471381186</v>
+        <v>-0.28166220370921385</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" si="3"/>
-        <v>-0.11778563015311881</v>
+        <v>-0.1170960187353605</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" si="3"/>
-        <v>-2.1424745581147035E-2</v>
+        <v>-2.1401819154628951E-2</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" si="3"/>
-        <v>-6.4366632337796076E-2</v>
+        <v>-6.4574454345860774E-2</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" si="3"/>
-        <v>0.10373870172555372</v>
+        <v>0.10427959320633842</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="I20" s="1">
         <f t="shared" si="3"/>
-        <v>-0.10087658271879704</v>
+        <v>-0.10037033191430371</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="I21" s="1">
         <f t="shared" si="3"/>
-        <v>-1.5564202334630019E-2</v>
+        <v>-1.5576323987538609E-2</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="I22" s="1">
         <f t="shared" si="3"/>
-        <v>0.26050420168067417</v>
+        <v>0.26394210302256477</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" si="3"/>
-        <v>0.81840014779235293</v>
+        <v>0.85331792352884661</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="I24" s="1">
         <f t="shared" si="3"/>
-        <v>8.0204156033540988E-2</v>
+        <v>7.9883805374002512E-2</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" si="3"/>
-        <v>0.76817180616740255</v>
+        <v>0.73975871669097337</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="I26" s="1">
         <f t="shared" si="3"/>
-        <v>0.12618296529968726</v>
+        <v>0.12698412698412972</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="I27" s="1">
         <f t="shared" si="3"/>
-        <v>3.6166365280291768E-2</v>
+        <v>3.6231884057973458E-2</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="I28" s="1">
         <f t="shared" si="3"/>
-        <v>6.7783353972496935E-2</v>
+        <v>6.8013864364660281E-2</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="I29" s="1">
         <f t="shared" si="3"/>
-        <v>-1.0805618921836352E-2</v>
+        <v>-1.0799784004316915E-2</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="I30" s="1">
         <f t="shared" si="3"/>
-        <v>5.004909879945646E-2</v>
+        <v>5.0174658621785995E-2</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="I31" s="1">
         <f t="shared" si="3"/>
-        <v>0.64824549223414729</v>
+        <v>0.62789401886756313</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="I32" s="1">
         <f t="shared" si="3"/>
-        <v>-2.5665988140545222E-2</v>
+        <v>-2.5633093207232109E-2</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="I33" s="1">
         <f t="shared" si="3"/>
-        <v>-0.75974675108297263</v>
+        <v>-0.78974714236231425</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="I34" s="1">
         <f t="shared" si="3"/>
-        <v>-0.1792037772293151</v>
+        <v>-0.18082399436955093</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="I35" s="1">
         <f t="shared" si="3"/>
-        <v>7.7356725737541918E-2</v>
+        <v>7.7657090650693969E-2</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="I36" s="1">
         <f t="shared" si="3"/>
-        <v>2.239571992908107E-2</v>
+        <v>2.2370669566569124E-2</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="I37" s="1">
         <f t="shared" si="3"/>
-        <v>8.5208958152313191E-2</v>
+        <v>8.4847469926597918E-2</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="I38" s="1">
         <f t="shared" si="3"/>
-        <v>1.0343935867599238E-2</v>
+        <v>1.0349288486418176E-2</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="I39" s="1">
         <f t="shared" si="3"/>
-        <v>0.13787510137875239</v>
+        <v>0.1388321763985314</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="I40" s="1">
         <f t="shared" si="3"/>
-        <v>0.29073740448530827</v>
+        <v>0.28657155103790377</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="I41" s="1">
         <f t="shared" si="3"/>
-        <v>-0.38108882521489923</v>
+        <v>-0.38849131006280074</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="I42" s="1">
         <f t="shared" si="3"/>
-        <v>-0.3571951398038351</v>
+        <v>-0.35092765712641993</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="I43" s="1">
         <f t="shared" si="3"/>
-        <v>0.60845651426607184</v>
+        <v>0.59049207673060988</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="I44" s="1">
         <f t="shared" si="3"/>
-        <v>6.1680801850427729E-2</v>
+        <v>6.149116064566084E-2</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="I45" s="1">
         <f t="shared" si="3"/>
-        <v>-2.1758997345402323E-2</v>
+        <v>-2.178269582643548E-2</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="I46" s="1">
         <f t="shared" si="3"/>
-        <v>-0.25802685347343601</v>
+        <v>-0.2547403607861195</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="I47" s="1">
         <f t="shared" si="3"/>
-        <v>-0.25656033557701641</v>
+        <v>-0.25331085961955169</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="I48" s="1">
         <f t="shared" si="3"/>
-        <v>-0.32899442139894314</v>
+        <v>-0.32367013791162558</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="I49" s="1">
         <f t="shared" si="3"/>
-        <v>-2.0760464853886024E-2</v>
+        <v>-2.0782037091417453E-2</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="I50" s="1">
         <f t="shared" si="3"/>
-        <v>-9.2599451811245265E-2</v>
+        <v>-9.217269476090402E-2</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="I51" s="1">
         <f t="shared" si="3"/>
-        <v>-0.27251568059158326</v>
+        <v>-0.26885235644679578</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="I52" s="1">
         <f t="shared" si="3"/>
-        <v>0.24229926536924801</v>
+        <v>0.2393989558130645</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="I53" s="1">
         <f t="shared" si="3"/>
-        <v>-0.14071294559099304</v>
+        <v>-0.14170996693433971</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="I54" s="1">
         <f t="shared" si="3"/>
-        <v>-0.26930815663210173</v>
+        <v>-0.26572999389126589</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="I55" s="1">
         <f t="shared" si="3"/>
-        <v>-0.13616557734204793</v>
+        <v>-0.13709898546750754</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="I56" s="1">
         <f t="shared" si="3"/>
-        <v>0.16362090947726526</v>
+        <v>0.16497054097482813</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
@@ -4065,7 +4065,7 @@
       </c>
       <c r="I57" s="1">
         <f t="shared" si="3"/>
-        <v>0.15924901517056456</v>
+        <v>0.1579910194578418</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="I58" s="1">
         <f t="shared" si="3"/>
-        <v>-0.13349814585908681</v>
+        <v>-0.13439522150323702</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="I59" s="1">
         <f t="shared" si="3"/>
-        <v>0.27266681445355884</v>
+        <v>0.27643555455669266</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="I60" s="1">
         <f t="shared" si="3"/>
-        <v>9.8972211648267625E-2</v>
+        <v>9.9464422341239117E-2</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="I61" s="1">
         <f t="shared" si="3"/>
-        <v>-3.3986928104573974E-2</v>
+        <v>-3.404478198245265E-2</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="I62" s="1">
         <f t="shared" si="3"/>
-        <v>-0.11092755123568304</v>
+        <v>-0.11154622873584519</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="I63" s="1">
         <f t="shared" si="3"/>
-        <v>-0.11963023382272912</v>
+        <v>-0.11891891891891831</v>
       </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="I64" s="1">
         <f t="shared" si="3"/>
-        <v>0.26754748142031454</v>
+        <v>0.27117509206561846</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="I65" s="1">
         <f t="shared" si="3"/>
-        <v>8.4961076444642181E-2</v>
+        <v>8.4601683937822816E-2</v>
       </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="I66" s="1">
         <f t="shared" si="3"/>
-        <v>-5.2910052910053122E-2</v>
+        <v>-5.2770448548812882E-2</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -4424,8 +4424,8 @@
         <v>0.53999999999999204</v>
       </c>
       <c r="I67" s="1">
-        <f t="shared" ref="I67:I130" si="8">($L$2/COUNT($B$2:$B$501)) * (H67 / B67)</f>
-        <v>4.9792531120331218E-2</v>
+        <f t="shared" ref="I67:I130" si="8">($L$2/COUNT($B$2:$B$501)) * (H67 / A67)</f>
+        <v>4.9916805324458496E-2</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="I68" s="1">
         <f t="shared" si="8"/>
-        <v>0.1386646405166663</v>
+        <v>0.13770986606300506</v>
       </c>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="I69" s="1">
         <f t="shared" si="8"/>
-        <v>0.548669447218471</v>
+        <v>0.5340194396798188</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="I70" s="1">
         <f t="shared" si="8"/>
-        <v>-0.40669856459330128</v>
+        <v>-0.39859320046893304</v>
       </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="I71" s="1">
         <f t="shared" si="8"/>
-        <v>-0.32299893905458077</v>
+        <v>-0.32830098250659107</v>
       </c>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="I72" s="1">
         <f t="shared" si="8"/>
-        <v>-0.14611872146118735</v>
+        <v>-0.14719411223551071</v>
       </c>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
@@ -4641,7 +4641,7 @@
       </c>
       <c r="I73" s="1">
         <f t="shared" si="8"/>
-        <v>3.1746031746032195E-2</v>
+        <v>3.1695721077654962E-2</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="I74" s="1">
         <f t="shared" si="8"/>
-        <v>-6.1307901907356854E-2</v>
+        <v>-6.112054329371807E-2</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="I75" s="1">
         <f t="shared" si="8"/>
-        <v>-4.1016495764601688E-2</v>
+        <v>-4.1100786275912078E-2</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="I76" s="1">
         <f t="shared" si="8"/>
-        <v>-1.934156378600822</v>
+        <v>-1.7636022514071286</v>
       </c>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
@@ -4785,7 +4785,7 @@
       </c>
       <c r="I77" s="1">
         <f t="shared" si="8"/>
-        <v>5.5325749741468103E-2</v>
+        <v>5.5479221216913031E-2</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
@@ -4821,7 +4821,7 @@
       </c>
       <c r="I78" s="1">
         <f t="shared" si="8"/>
-        <v>6.7344648141220306E-2</v>
+        <v>6.7118644067797217E-2</v>
       </c>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="I79" s="1">
         <f t="shared" si="8"/>
-        <v>-0.14873344178480077</v>
+        <v>-0.1498478108171383</v>
       </c>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="I80" s="1">
         <f t="shared" si="8"/>
-        <v>1.5550561797752802</v>
+        <v>1.68615984405458</v>
       </c>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
@@ -4929,7 +4929,7 @@
       </c>
       <c r="I81" s="1">
         <f t="shared" si="8"/>
-        <v>0.13817855540601093</v>
+        <v>0.13913986266714781</v>
       </c>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
@@ -4965,7 +4965,7 @@
       </c>
       <c r="I82" s="1">
         <f t="shared" si="8"/>
-        <v>8.6083213773314057E-2</v>
+        <v>8.5714285714285576E-2</v>
       </c>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="I83" s="1">
         <f t="shared" si="8"/>
-        <v>0.17509650204942409</v>
+        <v>0.17664298044883284</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="I84" s="1">
         <f t="shared" si="8"/>
-        <v>0.13507963309450918</v>
+        <v>0.13599816218699654</v>
       </c>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="I85" s="1">
         <f t="shared" si="8"/>
-        <v>0.13251155624037189</v>
+        <v>0.13339537769505408</v>
       </c>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="I86" s="1">
         <f t="shared" si="8"/>
-        <v>-0.11796287194222861</v>
+        <v>-0.11727118962601032</v>
       </c>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="I87" s="1">
         <f t="shared" si="8"/>
-        <v>-0.2283105022831057</v>
+        <v>-0.22573363431151308</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
@@ -5181,7 +5181,7 @@
       </c>
       <c r="I88" s="1">
         <f t="shared" si="8"/>
-        <v>-0.15325670498084307</v>
+        <v>-0.15444015444015458</v>
       </c>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="I89" s="1">
         <f t="shared" si="8"/>
-        <v>-9.7456388266245319E-3</v>
+        <v>-9.7503900156000693E-3</v>
       </c>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
@@ -5253,7 +5253,7 @@
       </c>
       <c r="I90" s="1">
         <f t="shared" si="8"/>
-        <v>0.21174927386863965</v>
+        <v>0.20953087335434739</v>
       </c>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="I91" s="1">
         <f t="shared" si="8"/>
-        <v>3.0707260460816374E-3</v>
+        <v>3.0702546505354624E-3</v>
       </c>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="I92" s="1">
         <f t="shared" si="8"/>
-        <v>4.2733699921445836E-2</v>
+        <v>4.2825203892055727E-2</v>
       </c>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
@@ -5361,7 +5361,7 @@
       </c>
       <c r="I93" s="1">
         <f t="shared" si="8"/>
-        <v>9.2592592592590617E-2</v>
+        <v>9.2165898617509567E-2</v>
       </c>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="I94" s="1">
         <f t="shared" si="8"/>
-        <v>0.15239623019851431</v>
+        <v>0.15356637704586601</v>
       </c>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="I95" s="1">
         <f t="shared" si="8"/>
-        <v>-5.0320795068587833E-3</v>
+        <v>-5.0308137341240674E-3</v>
       </c>
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="I96" s="1">
         <f t="shared" si="8"/>
-        <v>-4.3227665706053506E-2</v>
+        <v>-4.3321299638990819E-2</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
@@ -5505,7 +5505,7 @@
       </c>
       <c r="I97" s="1">
         <f t="shared" si="8"/>
-        <v>-0.22203839958204635</v>
+        <v>-0.22453112617768878</v>
       </c>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="I98" s="1">
         <f t="shared" si="8"/>
-        <v>-0.14131897711978283</v>
+        <v>-0.14232463571670437</v>
       </c>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="I99" s="1">
         <f t="shared" si="8"/>
-        <v>0.15098652550529301</v>
+        <v>0.1521350425796279</v>
       </c>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
@@ -5613,7 +5613,7 @@
       </c>
       <c r="I100" s="1">
         <f t="shared" si="8"/>
-        <v>9.4760312151613485E-2</v>
+        <v>9.4313453536751524E-2</v>
       </c>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="I101" s="1">
         <f t="shared" si="8"/>
-        <v>0.57476863127131128</v>
+        <v>0.59177532597793481</v>
       </c>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
@@ -5685,7 +5685,7 @@
       </c>
       <c r="I102" s="1">
         <f t="shared" si="8"/>
-        <v>-0.1831750339213023</v>
+        <v>-0.18151260504201652</v>
       </c>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="I103" s="1">
         <f t="shared" si="8"/>
-        <v>0.1305057096247961</v>
+        <v>0.12965964343598055</v>
       </c>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="I104" s="1">
         <f t="shared" si="8"/>
-        <v>0.36722900549911697</v>
+        <v>0.3740979870869755</v>
       </c>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="I105" s="1">
         <f t="shared" si="8"/>
-        <v>-2.2990707922215643E-2</v>
+        <v>-2.2964309635442451E-2</v>
       </c>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="I106" s="1">
         <f t="shared" si="8"/>
-        <v>-5.4855101737076681E-2</v>
+        <v>-5.5005969640114429E-2</v>
       </c>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="I107" s="1">
         <f t="shared" si="8"/>
-        <v>0.12736714867708154</v>
+        <v>0.12656116196047335</v>
       </c>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
@@ -5901,7 +5901,7 @@
       </c>
       <c r="I108" s="1">
         <f t="shared" si="8"/>
-        <v>0.61007880426880745</v>
+        <v>0.59201986568090803</v>
       </c>
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="I109" s="1">
         <f t="shared" si="8"/>
-        <v>8.5142613878229131E-3</v>
+        <v>8.5178875638824616E-3</v>
       </c>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="I110" s="1">
         <f t="shared" si="8"/>
-        <v>1.1675423234092678E-2</v>
+        <v>1.1682242990654649E-2</v>
       </c>
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="I111" s="1">
         <f t="shared" si="8"/>
-        <v>-4.4865403788633434E-2</v>
+        <v>-4.4764983834866295E-2</v>
       </c>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="I112" s="1">
         <f t="shared" si="8"/>
-        <v>-0.43245018611780034</v>
+        <v>-0.4232974334244215</v>
       </c>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="I113" s="1">
         <f t="shared" si="8"/>
-        <v>-0.16181342632955487</v>
+        <v>-0.16313328411208333</v>
       </c>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="I114" s="1">
         <f t="shared" si="8"/>
-        <v>-0.34799737360472821</v>
+        <v>-0.35415970598062224</v>
       </c>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
@@ -6153,7 +6153,7 @@
       </c>
       <c r="I115" s="1">
         <f t="shared" si="8"/>
-        <v>0.1143674052894926</v>
+        <v>0.11371712864250189</v>
       </c>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="I116" s="1">
         <f t="shared" si="8"/>
-        <v>0.29228687415426591</v>
+        <v>0.29662180719582881</v>
       </c>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="I117" s="1">
         <f t="shared" si="8"/>
-        <v>-0.29913884272548996</v>
+        <v>-0.29473057457576929</v>
       </c>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="I118" s="1">
         <f t="shared" si="8"/>
-        <v>5.3550083672005949E-2</v>
+        <v>5.3407085975871661E-2</v>
       </c>
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="I119" s="1">
         <f t="shared" si="8"/>
-        <v>2.354128131831185E-2</v>
+        <v>2.3569023569023666E-2</v>
       </c>
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
@@ -6333,7 +6333,7 @@
       </c>
       <c r="I120" s="1">
         <f t="shared" si="8"/>
-        <v>0.27488546438983907</v>
+        <v>0.27871621621621778</v>
       </c>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
@@ -6369,7 +6369,7 @@
       </c>
       <c r="I121" s="1">
         <f t="shared" si="8"/>
-        <v>-0.31648527742538235</v>
+        <v>-0.31155514657551941</v>
       </c>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
@@ -6440,7 +6440,7 @@
       </c>
       <c r="I123" s="1">
         <f t="shared" si="8"/>
-        <v>-0.23521026372060005</v>
+        <v>-0.23247622402254445</v>
       </c>
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
@@ -6476,7 +6476,7 @@
       </c>
       <c r="I124" s="1">
         <f t="shared" si="8"/>
-        <v>-1.3291686050363402E-3</v>
+        <v>-1.3290802764474887E-3</v>
       </c>
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
@@ -6512,7 +6512,7 @@
       </c>
       <c r="I125" s="1">
         <f t="shared" si="8"/>
-        <v>0.39844286695672293</v>
+        <v>0.40654205607476851</v>
       </c>
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
@@ -6548,7 +6548,7 @@
       </c>
       <c r="I126" s="1">
         <f t="shared" si="8"/>
-        <v>5.2657561296691323E-2</v>
+        <v>5.251928442474859E-2</v>
       </c>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
@@ -6584,7 +6584,7 @@
       </c>
       <c r="I127" s="1">
         <f t="shared" si="8"/>
-        <v>-4.5641259698767686E-2</v>
+        <v>-4.5745654162854532E-2</v>
       </c>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
@@ -6620,7 +6620,7 @@
       </c>
       <c r="I128" s="1">
         <f t="shared" si="8"/>
-        <v>-6.1481709191516395E-2</v>
+        <v>-6.1671292013568559E-2</v>
       </c>
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="I129" s="1">
         <f t="shared" si="8"/>
-        <v>-4.0370458323439017E-2</v>
+        <v>-4.0289133783624059E-2</v>
       </c>
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
@@ -6692,7 +6692,7 @@
       </c>
       <c r="I130" s="1">
         <f t="shared" si="8"/>
-        <v>0.11871168628977317</v>
+        <v>0.11942051683633506</v>
       </c>
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
@@ -6727,8 +6727,8 @@
         <v>1.1500000000000057</v>
       </c>
       <c r="I131" s="1">
-        <f t="shared" ref="I131:I194" si="13">($L$2/COUNT($B$2:$B$501)) * (H131 / B131)</f>
-        <v>0.15120636381566047</v>
+        <f t="shared" ref="I131:I194" si="13">($L$2/COUNT($B$2:$B$501)) * (H131 / A131)</f>
+        <v>0.15235824059353545</v>
       </c>
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
@@ -6764,7 +6764,7 @@
       </c>
       <c r="I132" s="1">
         <f t="shared" si="13"/>
-        <v>-0.18079283463260962</v>
+        <v>-0.18244204535944486</v>
       </c>
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
@@ -6800,7 +6800,7 @@
       </c>
       <c r="I133" s="1">
         <f t="shared" si="13"/>
-        <v>0.27232735144193682</v>
+        <v>0.26866905483604142</v>
       </c>
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
@@ -6836,7 +6836,7 @@
       </c>
       <c r="I134" s="1">
         <f t="shared" si="13"/>
-        <v>9.0897924087947501E-2</v>
+        <v>9.1312931885486254E-2</v>
       </c>
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
@@ -6872,7 +6872,7 @@
       </c>
       <c r="I135" s="1">
         <f t="shared" si="13"/>
-        <v>-0.11139240506329057</v>
+        <v>-0.11201629327902182</v>
       </c>
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
@@ -6908,7 +6908,7 @@
       </c>
       <c r="I136" s="1">
         <f t="shared" si="13"/>
-        <v>0.26382047071702208</v>
+        <v>0.26734705197182285</v>
       </c>
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
@@ -6944,7 +6944,7 @@
       </c>
       <c r="I137" s="1">
         <f t="shared" si="13"/>
-        <v>-0.65765584022594359</v>
+        <v>-0.63671875000000044</v>
       </c>
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
@@ -6980,7 +6980,7 @@
       </c>
       <c r="I138" s="1">
         <f t="shared" si="13"/>
-        <v>0.17187172500523856</v>
+        <v>0.17040731504571763</v>
       </c>
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
@@ -7016,7 +7016,7 @@
       </c>
       <c r="I139" s="1">
         <f t="shared" si="13"/>
-        <v>6.6565809379729057E-2</v>
+        <v>6.6344993968638272E-2</v>
       </c>
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
@@ -7052,7 +7052,7 @@
       </c>
       <c r="I140" s="1">
         <f t="shared" si="13"/>
-        <v>0.25085859340003092</v>
+        <v>0.25404506275518024</v>
       </c>
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
@@ -7088,7 +7088,7 @@
       </c>
       <c r="I141" s="1">
         <f t="shared" si="13"/>
-        <v>0.11746791385686453</v>
+        <v>0.11678200692041658</v>
       </c>
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
@@ -7124,7 +7124,7 @@
       </c>
       <c r="I142" s="1">
         <f t="shared" si="13"/>
-        <v>0.75357297531398959</v>
+        <v>0.72621035058430805</v>
       </c>
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
@@ -7160,7 +7160,7 @@
       </c>
       <c r="I143" s="1">
         <f t="shared" si="13"/>
-        <v>-0.19611688566385566</v>
+        <v>-0.19421246844047388</v>
       </c>
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
@@ -7196,7 +7196,7 @@
       </c>
       <c r="I144" s="1">
         <f t="shared" si="13"/>
-        <v>-0.35832972113856365</v>
+        <v>-0.35202271114265427</v>
       </c>
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
@@ -7232,7 +7232,7 @@
       </c>
       <c r="I145" s="1">
         <f t="shared" si="13"/>
-        <v>-2.5835024912342935E-2</v>
+        <v>-2.5868440502584321E-2</v>
       </c>
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
@@ -7268,7 +7268,7 @@
       </c>
       <c r="I146" s="1">
         <f t="shared" si="13"/>
-        <v>4.3173232595790784E-2</v>
+        <v>4.3080236941303349E-2</v>
       </c>
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
@@ -7304,7 +7304,7 @@
       </c>
       <c r="I147" s="1">
         <f t="shared" si="13"/>
-        <v>0.26216284345853091</v>
+        <v>0.25877083851704208</v>
       </c>
       <c r="J147" s="1"/>
       <c r="K147" s="1"/>
@@ -7340,7 +7340,7 @@
       </c>
       <c r="I148" s="1">
         <f t="shared" si="13"/>
-        <v>0.1735035320361886</v>
+        <v>0.17201130359995154</v>
       </c>
       <c r="J148" s="1"/>
       <c r="K148" s="1"/>
@@ -7411,7 +7411,7 @@
       </c>
       <c r="I150" s="1">
         <f t="shared" si="13"/>
-        <v>-0.6436106289224186</v>
+        <v>-0.66501103752759283</v>
       </c>
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
@@ -7447,7 +7447,7 @@
       </c>
       <c r="I151" s="1">
         <f t="shared" si="13"/>
-        <v>-1.9310344827584324E-2</v>
+        <v>-1.9329007317408026E-2</v>
       </c>
       <c r="J151" s="1"/>
       <c r="K151" s="1"/>
@@ -7483,7 +7483,7 @@
       </c>
       <c r="I152" s="1">
         <f t="shared" si="13"/>
-        <v>-2.831078955646537E-2</v>
+        <v>-2.8270771163814483E-2</v>
       </c>
       <c r="J152" s="1"/>
       <c r="K152" s="1"/>
@@ -7519,7 +7519,7 @@
       </c>
       <c r="I153" s="1">
         <f t="shared" si="13"/>
-        <v>0.18018018018018034</v>
+        <v>0.17857142857142874</v>
       </c>
       <c r="J153" s="1"/>
       <c r="K153" s="1"/>
@@ -7555,7 +7555,7 @@
       </c>
       <c r="I154" s="1">
         <f t="shared" si="13"/>
-        <v>6.9139493599926105E-2</v>
+        <v>6.890130353817589E-2</v>
       </c>
       <c r="J154" s="1"/>
       <c r="K154" s="1"/>
@@ -7591,7 +7591,7 @@
       </c>
       <c r="I155" s="1">
         <f t="shared" si="13"/>
-        <v>-4.4166359955835318E-3</v>
+        <v>-4.4156608772447951E-3</v>
       </c>
       <c r="J155" s="1"/>
       <c r="K155" s="1"/>
@@ -7627,7 +7627,7 @@
       </c>
       <c r="I156" s="1">
         <f t="shared" si="13"/>
-        <v>7.7487343733856795E-2</v>
+        <v>7.7788725820671062E-2</v>
       </c>
       <c r="J156" s="1"/>
       <c r="K156" s="1"/>
@@ -7663,7 +7663,7 @@
       </c>
       <c r="I157" s="1">
         <f t="shared" si="13"/>
-        <v>-8.8764307404810894E-2</v>
+        <v>-8.8372093023254758E-2</v>
       </c>
       <c r="J157" s="1"/>
       <c r="K157" s="1"/>
@@ -7699,7 +7699,7 @@
       </c>
       <c r="I158" s="1">
         <f t="shared" si="13"/>
-        <v>0.191787003610107</v>
+        <v>0.19364392299806227</v>
       </c>
       <c r="J158" s="1"/>
       <c r="K158" s="1"/>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="I159" s="1">
         <f t="shared" si="13"/>
-        <v>0.15805180852333783</v>
+        <v>0.15931077633922136</v>
       </c>
       <c r="J159" s="1"/>
       <c r="K159" s="1"/>
@@ -7771,7 +7771,7 @@
       </c>
       <c r="I160" s="1">
         <f t="shared" si="13"/>
-        <v>-4.6847184484212497E-2</v>
+        <v>-4.6737707982800525E-2</v>
       </c>
       <c r="J160" s="1"/>
       <c r="K160" s="1"/>
@@ -7807,7 +7807,7 @@
       </c>
       <c r="I161" s="1">
         <f t="shared" si="13"/>
-        <v>-4.6185109920561601E-2</v>
+        <v>-4.6078702423739744E-2</v>
       </c>
       <c r="J161" s="1"/>
       <c r="K161" s="1"/>
@@ -7843,7 +7843,7 @@
       </c>
       <c r="I162" s="1">
         <f t="shared" si="13"/>
-        <v>0.6390328151986191</v>
+        <v>0.66012488849241835</v>
       </c>
       <c r="J162" s="1"/>
       <c r="K162" s="1"/>
@@ -7879,7 +7879,7 @@
       </c>
       <c r="I163" s="1">
         <f t="shared" si="13"/>
-        <v>-4.6608807457410202E-2</v>
+        <v>-4.6500440952458311E-2</v>
       </c>
       <c r="J163" s="1"/>
       <c r="K163" s="1"/>
@@ -7915,7 +7915,7 @@
       </c>
       <c r="I164" s="1">
         <f t="shared" si="13"/>
-        <v>-0.23253378024510304</v>
+        <v>-0.22986125491820242</v>
       </c>
       <c r="J164" s="1"/>
       <c r="K164" s="1"/>
@@ -7951,7 +7951,7 @@
       </c>
       <c r="I165" s="1">
         <f t="shared" si="13"/>
-        <v>-9.8262539640001284E-2</v>
+        <v>-9.8747699627451363E-2</v>
       </c>
       <c r="J165" s="1"/>
       <c r="K165" s="1"/>
@@ -7987,7 +7987,7 @@
       </c>
       <c r="I166" s="1">
         <f t="shared" si="13"/>
-        <v>-5.7833859095688452E-2</v>
+        <v>-5.800158186132319E-2</v>
       </c>
       <c r="J166" s="1"/>
       <c r="K166" s="1"/>
@@ -8023,7 +8023,7 @@
       </c>
       <c r="I167" s="1">
         <f t="shared" si="13"/>
-        <v>0.42196375439545636</v>
+        <v>0.43105830339872964</v>
       </c>
       <c r="J167" s="1"/>
       <c r="K167" s="1"/>
@@ -8059,7 +8059,7 @@
       </c>
       <c r="I168" s="1">
         <f t="shared" si="13"/>
-        <v>-0.24488726891764875</v>
+        <v>-0.24192505067057471</v>
       </c>
       <c r="J168" s="1"/>
       <c r="K168" s="1"/>
@@ -8095,7 +8095,7 @@
       </c>
       <c r="I169" s="1">
         <f t="shared" si="13"/>
-        <v>8.3819787456967859E-2</v>
+        <v>8.3469965717692995E-2</v>
       </c>
       <c r="J169" s="1"/>
       <c r="K169" s="1"/>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="I170" s="1">
         <f t="shared" si="13"/>
-        <v>-0.12786114147537228</v>
+        <v>-0.12868382450993512</v>
       </c>
       <c r="J170" s="1"/>
       <c r="K170" s="1"/>
@@ -8167,7 +8167,7 @@
       </c>
       <c r="I171" s="1">
         <f t="shared" si="13"/>
-        <v>-1.8535681186283202E-2</v>
+        <v>-1.8552875695732444E-2</v>
       </c>
       <c r="J171" s="1"/>
       <c r="K171" s="1"/>
@@ -8203,7 +8203,7 @@
       </c>
       <c r="I172" s="1">
         <f t="shared" si="13"/>
-        <v>-7.5652869717030669E-2</v>
+        <v>-7.5940124132896719E-2</v>
       </c>
       <c r="J172" s="1"/>
       <c r="K172" s="1"/>
@@ -8239,7 +8239,7 @@
       </c>
       <c r="I173" s="1">
         <f t="shared" si="13"/>
-        <v>0.10056772100567796</v>
+        <v>0.10006455777921314</v>
       </c>
       <c r="J173" s="1"/>
       <c r="K173" s="1"/>
@@ -8275,7 +8275,7 @@
       </c>
       <c r="I174" s="1">
         <f t="shared" si="13"/>
-        <v>6.8210885320447598E-2</v>
+        <v>6.797903979606143E-2</v>
       </c>
       <c r="J174" s="1"/>
       <c r="K174" s="1"/>
@@ -8311,7 +8311,7 @@
       </c>
       <c r="I175" s="1">
         <f t="shared" si="13"/>
-        <v>-9.823182711199965E-3</v>
+        <v>-9.8183603338257864E-3</v>
       </c>
       <c r="J175" s="1"/>
       <c r="K175" s="1"/>
@@ -8347,7 +8347,7 @@
       </c>
       <c r="I176" s="1">
         <f t="shared" si="13"/>
-        <v>1.5051425704490914E-2</v>
+        <v>1.5062761506276723E-2</v>
       </c>
       <c r="J176" s="1"/>
       <c r="K176" s="1"/>
@@ -8383,7 +8383,7 @@
       </c>
       <c r="I177" s="1">
         <f t="shared" si="13"/>
-        <v>-0.26420737786639786</v>
+        <v>-0.26774437989390953</v>
       </c>
       <c r="J177" s="1"/>
       <c r="K177" s="1"/>
@@ -8419,7 +8419,7 @@
       </c>
       <c r="I178" s="1">
         <f t="shared" si="13"/>
-        <v>-9.2702638459710149E-2</v>
+        <v>-9.2274931976813107E-2</v>
       </c>
       <c r="J178" s="1"/>
       <c r="K178" s="1"/>
@@ -8455,7 +8455,7 @@
       </c>
       <c r="I179" s="1">
         <f t="shared" si="13"/>
-        <v>-0.31152647975077696</v>
+        <v>-0.31645569620252972</v>
       </c>
       <c r="J179" s="1"/>
       <c r="K179" s="1"/>
@@ -8491,7 +8491,7 @@
       </c>
       <c r="I180" s="1">
         <f t="shared" si="13"/>
-        <v>-2.8751520513103052E-2</v>
+        <v>-2.8710247349822315E-2</v>
       </c>
       <c r="J180" s="1"/>
       <c r="K180" s="1"/>
@@ -8527,7 +8527,7 @@
       </c>
       <c r="I181" s="1">
         <f t="shared" si="13"/>
-        <v>7.6679005817029675E-2</v>
+        <v>7.6386145133677391E-2</v>
       </c>
       <c r="J181" s="1"/>
       <c r="K181" s="1"/>
@@ -8563,7 +8563,7 @@
       </c>
       <c r="I182" s="1">
         <f t="shared" si="13"/>
-        <v>-0.45677694770544297</v>
+        <v>-0.44657762938230394</v>
       </c>
       <c r="J182" s="1"/>
       <c r="K182" s="1"/>
@@ -8599,7 +8599,7 @@
       </c>
       <c r="I183" s="1">
         <f t="shared" si="13"/>
-        <v>0.30738916256157556</v>
+        <v>0.30273627013390181</v>
       </c>
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="I184" s="1">
         <f t="shared" si="13"/>
-        <v>-0.34824046920821111</v>
+        <v>-0.35441149039358327</v>
       </c>
       <c r="J184" s="1"/>
       <c r="K184" s="1"/>
@@ -8671,7 +8671,7 @@
       </c>
       <c r="I185" s="1">
         <f t="shared" si="13"/>
-        <v>8.1651168065320801E-2</v>
+        <v>8.1319177772757947E-2</v>
       </c>
       <c r="J185" s="1"/>
       <c r="K185" s="1"/>
@@ -8707,7 +8707,7 @@
       </c>
       <c r="I186" s="1">
         <f t="shared" si="13"/>
-        <v>-0.1647554411420539</v>
+        <v>-0.16340931247388615</v>
       </c>
       <c r="J186" s="1"/>
       <c r="K186" s="1"/>
@@ -8743,7 +8743,7 @@
       </c>
       <c r="I187" s="1">
         <f t="shared" si="13"/>
-        <v>-9.0515545060998376E-2</v>
+        <v>-9.092706068392839E-2</v>
       </c>
       <c r="J187" s="1"/>
       <c r="K187" s="1"/>
@@ -8779,7 +8779,7 @@
       </c>
       <c r="I188" s="1">
         <f t="shared" si="13"/>
-        <v>-2.9463050928988582E-2</v>
+        <v>-2.9419711206508905E-2</v>
       </c>
       <c r="J188" s="1"/>
       <c r="K188" s="1"/>
@@ -8815,7 +8815,7 @@
       </c>
       <c r="I189" s="1">
         <f t="shared" si="13"/>
-        <v>-9.9612617598226608E-2</v>
+        <v>-0.1001112347052255</v>
       </c>
       <c r="J189" s="1"/>
       <c r="K189" s="1"/>
@@ -8851,7 +8851,7 @@
       </c>
       <c r="I190" s="1">
         <f t="shared" si="13"/>
-        <v>-7.7202543142598418E-2</v>
+        <v>-7.7501709596536003E-2</v>
       </c>
       <c r="J190" s="1"/>
       <c r="K190" s="1"/>
@@ -8887,7 +8887,7 @@
       </c>
       <c r="I191" s="1">
         <f t="shared" si="13"/>
-        <v>-0.19509022923101982</v>
+        <v>-0.19320560296248637</v>
       </c>
       <c r="J191" s="1"/>
       <c r="K191" s="1"/>
@@ -8923,7 +8923,7 @@
       </c>
       <c r="I192" s="1">
         <f t="shared" si="13"/>
-        <v>-3.6515388628061127E-2</v>
+        <v>-3.6448841447536157E-2</v>
       </c>
       <c r="J192" s="1"/>
       <c r="K192" s="1"/>
@@ -8959,7 +8959,7 @@
       </c>
       <c r="I193" s="1">
         <f t="shared" si="13"/>
-        <v>-7.1925197794293252E-2</v>
+        <v>-7.166746297181012E-2</v>
       </c>
       <c r="J193" s="1"/>
       <c r="K193" s="1"/>
@@ -8995,7 +8995,7 @@
       </c>
       <c r="I194" s="1">
         <f t="shared" si="13"/>
-        <v>9.1300149240630374E-2</v>
+        <v>9.0885257362581517E-2</v>
       </c>
       <c r="J194" s="1"/>
       <c r="K194" s="1"/>
@@ -9030,8 +9030,8 @@
         <v>3.6400000000000148</v>
       </c>
       <c r="I195" s="1">
-        <f t="shared" ref="I195:I258" si="18">($L$2/COUNT($B$2:$B$501)) * (H195 / B195)</f>
-        <v>0.37133384340729553</v>
+        <f t="shared" ref="I195:I258" si="18">($L$2/COUNT($B$2:$B$501)) * (H195 / A195)</f>
+        <v>0.37835871316459796</v>
       </c>
       <c r="J195" s="1"/>
       <c r="K195" s="1"/>
@@ -9067,7 +9067,7 @@
       </c>
       <c r="I196" s="1">
         <f t="shared" si="18"/>
-        <v>-5.9545962039447925E-2</v>
+        <v>-5.9723777528927428E-2</v>
       </c>
       <c r="J196" s="1"/>
       <c r="K196" s="1"/>
@@ -9103,7 +9103,7 @@
       </c>
       <c r="I197" s="1">
         <f t="shared" si="18"/>
-        <v>-0.13197360527894542</v>
+        <v>-0.13110846245530514</v>
       </c>
       <c r="J197" s="1"/>
       <c r="K197" s="1"/>
@@ -9139,7 +9139,7 @@
       </c>
       <c r="I198" s="1">
         <f t="shared" si="18"/>
-        <v>0.20510437755135741</v>
+        <v>0.20302233902759365</v>
       </c>
       <c r="J198" s="1"/>
       <c r="K198" s="1"/>
@@ -9175,7 +9175,7 @@
       </c>
       <c r="I199" s="1">
         <f t="shared" si="18"/>
-        <v>5.4506039021368566E-2</v>
+        <v>5.4357897337698163E-2</v>
       </c>
       <c r="J199" s="1"/>
       <c r="K199" s="1"/>
@@ -9211,7 +9211,7 @@
       </c>
       <c r="I200" s="1">
         <f t="shared" si="18"/>
-        <v>-0.22485668169421835</v>
+        <v>-0.2223567615168705</v>
       </c>
       <c r="J200" s="1"/>
       <c r="K200" s="1"/>
@@ -9247,7 +9247,7 @@
       </c>
       <c r="I201" s="1">
         <f t="shared" si="18"/>
-        <v>-8.7739032620922502E-2</v>
+        <v>-8.7355806921267903E-2</v>
       </c>
       <c r="J201" s="1"/>
       <c r="K201" s="1"/>
@@ -9283,7 +9283,7 @@
       </c>
       <c r="I202" s="1">
         <f t="shared" si="18"/>
-        <v>0.16284233900814127</v>
+        <v>0.16417910447761111</v>
       </c>
       <c r="J202" s="1"/>
       <c r="K202" s="1"/>
@@ -9319,7 +9319,7 @@
       </c>
       <c r="I203" s="1">
         <f t="shared" si="18"/>
-        <v>-1.1534965152688459</v>
+        <v>-1.2240960411604971</v>
       </c>
       <c r="J203" s="1"/>
       <c r="K203" s="1"/>
@@ -9355,7 +9355,7 @@
       </c>
       <c r="I204" s="1">
         <f t="shared" si="18"/>
-        <v>-0.34253521126760472</v>
+        <v>-0.34850395506133119</v>
       </c>
       <c r="J204" s="1"/>
       <c r="K204" s="1"/>
@@ -9391,7 +9391,7 @@
       </c>
       <c r="I205" s="1">
         <f t="shared" si="18"/>
-        <v>8.7450808919985832E-3</v>
+        <v>8.7489063867019941E-3</v>
       </c>
       <c r="J205" s="1"/>
       <c r="K205" s="1"/>
@@ -9427,7 +9427,7 @@
       </c>
       <c r="I206" s="1">
         <f t="shared" si="18"/>
-        <v>0.26876314105494081</v>
+        <v>0.26519935053220256</v>
       </c>
       <c r="J206" s="1"/>
       <c r="K206" s="1"/>
@@ -9463,7 +9463,7 @@
       </c>
       <c r="I207" s="1">
         <f t="shared" si="18"/>
-        <v>3.4180730613116127E-2</v>
+        <v>3.4122414160801147E-2</v>
       </c>
       <c r="J207" s="1"/>
       <c r="K207" s="1"/>
@@ -9499,7 +9499,7 @@
       </c>
       <c r="I208" s="1">
         <f t="shared" si="18"/>
-        <v>8.349146110056882E-2</v>
+        <v>8.3144368858654144E-2</v>
       </c>
       <c r="J208" s="1"/>
       <c r="K208" s="1"/>
@@ -9535,7 +9535,7 @@
       </c>
       <c r="I209" s="1">
         <f t="shared" si="18"/>
-        <v>1.9274786170340511E-2</v>
+        <v>1.9256228186303594E-2</v>
       </c>
       <c r="J209" s="1"/>
       <c r="K209" s="1"/>
@@ -9571,7 +9571,7 @@
       </c>
       <c r="I210" s="1">
         <f t="shared" si="18"/>
-        <v>4.8626306832020988E-3</v>
+        <v>4.863813229574473E-3</v>
       </c>
       <c r="J210" s="1"/>
       <c r="K210" s="1"/>
@@ -9607,7 +9607,7 @@
       </c>
       <c r="I211" s="1">
         <f t="shared" si="18"/>
-        <v>-8.6042652572052326E-3</v>
+        <v>-8.6005651799967043E-3</v>
       </c>
       <c r="J211" s="1"/>
       <c r="K211" s="1"/>
@@ -9643,7 +9643,7 @@
       </c>
       <c r="I212" s="1">
         <f t="shared" si="18"/>
-        <v>-0.55162659123054991</v>
+        <v>-0.53682037164487106</v>
       </c>
       <c r="J212" s="1"/>
       <c r="K212" s="1"/>
@@ -9679,7 +9679,7 @@
       </c>
       <c r="I213" s="1">
         <f t="shared" si="18"/>
-        <v>7.4364385488893653E-2</v>
+        <v>7.4088906688023703E-2</v>
       </c>
       <c r="J213" s="1"/>
       <c r="K213" s="1"/>
@@ -9715,7 +9715,7 @@
       </c>
       <c r="I214" s="1">
         <f t="shared" si="18"/>
-        <v>3.9530574428658823E-2</v>
+        <v>3.960886248297972E-2</v>
       </c>
       <c r="J214" s="1"/>
       <c r="K214" s="1"/>
@@ -9751,7 +9751,7 @@
       </c>
       <c r="I215" s="1">
         <f t="shared" si="18"/>
-        <v>-0.27836034318398301</v>
+        <v>-0.28228924980664938</v>
       </c>
       <c r="J215" s="1"/>
       <c r="K215" s="1"/>
@@ -9787,7 +9787,7 @@
       </c>
       <c r="I216" s="1">
         <f t="shared" si="18"/>
-        <v>0.19314653260387488</v>
+        <v>0.19129909476170076</v>
       </c>
       <c r="J216" s="1"/>
       <c r="K216" s="1"/>
@@ -9823,7 +9823,7 @@
       </c>
       <c r="I217" s="1">
         <f t="shared" si="18"/>
-        <v>3.5893754486719817E-2</v>
+        <v>3.5958288385473366E-2</v>
       </c>
       <c r="J217" s="1"/>
       <c r="K217" s="1"/>
@@ -9859,7 +9859,7 @@
       </c>
       <c r="I218" s="1">
         <f t="shared" si="18"/>
-        <v>-1.28309880466031</v>
+        <v>-1.2057443480733669</v>
       </c>
       <c r="J218" s="1"/>
       <c r="K218" s="1"/>
@@ -9895,7 +9895,7 @@
       </c>
       <c r="I219" s="1">
         <f t="shared" si="18"/>
-        <v>-1.2861736334407155E-2</v>
+        <v>-1.2870012870014881E-2</v>
       </c>
       <c r="J219" s="1"/>
       <c r="K219" s="1"/>
@@ -9931,7 +9931,7 @@
       </c>
       <c r="I220" s="1">
         <f t="shared" si="18"/>
-        <v>0.56061175880656633</v>
+        <v>0.54532595175962495</v>
       </c>
       <c r="J220" s="1"/>
       <c r="K220" s="1"/>
@@ -9967,7 +9967,7 @@
       </c>
       <c r="I221" s="1">
         <f t="shared" si="18"/>
-        <v>0.13618967145484415</v>
+        <v>0.13712341106996342</v>
       </c>
       <c r="J221" s="1"/>
       <c r="K221" s="1"/>
@@ -10003,7 +10003,7 @@
       </c>
       <c r="I222" s="1">
         <f t="shared" si="18"/>
-        <v>6.6421197025482576E-2</v>
+        <v>6.6642520825784785E-2</v>
       </c>
       <c r="J222" s="1"/>
       <c r="K222" s="1"/>
@@ -10039,7 +10039,7 @@
       </c>
       <c r="I223" s="1">
         <f t="shared" si="18"/>
-        <v>-0.10458167330677451</v>
+        <v>-0.10513141426783641</v>
       </c>
       <c r="J223" s="1"/>
       <c r="K223" s="1"/>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="I224" s="1">
         <f t="shared" si="18"/>
-        <v>-0.10287015587577072</v>
+        <v>-0.10234375000000018</v>
       </c>
       <c r="J224" s="1"/>
       <c r="K224" s="1"/>
@@ -10111,7 +10111,7 @@
       </c>
       <c r="I225" s="1">
         <f t="shared" si="18"/>
-        <v>-0.14455782312925072</v>
+        <v>-0.14561027837259002</v>
       </c>
       <c r="J225" s="1"/>
       <c r="K225" s="1"/>
@@ -10147,7 +10147,7 @@
       </c>
       <c r="I226" s="1">
         <f t="shared" si="18"/>
-        <v>0.10627780523974112</v>
+        <v>0.10571604179471239</v>
       </c>
       <c r="J226" s="1"/>
       <c r="K226" s="1"/>
@@ -10183,7 +10183,7 @@
       </c>
       <c r="I227" s="1">
         <f t="shared" si="18"/>
-        <v>1.0730680948737565</v>
+        <v>1.0184260688027593</v>
       </c>
       <c r="J227" s="1"/>
       <c r="K227" s="1"/>
@@ -10219,7 +10219,7 @@
       </c>
       <c r="I228" s="1">
         <f t="shared" si="18"/>
-        <v>9.7912909044063287E-2</v>
+        <v>9.8394614189541596E-2</v>
       </c>
       <c r="J228" s="1"/>
       <c r="K228" s="1"/>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="I229" s="1">
         <f t="shared" si="18"/>
-        <v>-0.34000548395941732</v>
+        <v>-0.34588563458856197</v>
       </c>
       <c r="J229" s="1"/>
       <c r="K229" s="1"/>
@@ -10291,7 +10291,7 @@
       </c>
       <c r="I230" s="1">
         <f t="shared" si="18"/>
-        <v>6.432936635574231E-2</v>
+        <v>6.4123116383457149E-2</v>
       </c>
       <c r="J230" s="1"/>
       <c r="K230" s="1"/>
@@ -10327,7 +10327,7 @@
       </c>
       <c r="I231" s="1">
         <f t="shared" si="18"/>
-        <v>0.19461288957833811</v>
+        <v>0.19652520649387575</v>
       </c>
       <c r="J231" s="1"/>
       <c r="K231" s="1"/>
@@ -10363,7 +10363,7 @@
       </c>
       <c r="I232" s="1">
         <f t="shared" si="18"/>
-        <v>0.31710079275198316</v>
+        <v>0.32220943613348813</v>
       </c>
       <c r="J232" s="1"/>
       <c r="K232" s="1"/>
@@ -10399,7 +10399,7 @@
       </c>
       <c r="I233" s="1">
         <f t="shared" si="18"/>
-        <v>2.3052856907624784E-2</v>
+        <v>2.3079459281240573E-2</v>
       </c>
       <c r="J233" s="1"/>
       <c r="K233" s="1"/>
@@ -10435,7 +10435,7 @@
       </c>
       <c r="I234" s="1">
         <f t="shared" si="18"/>
-        <v>-0.23861894287808877</v>
+        <v>-0.24150026983270137</v>
       </c>
       <c r="J234" s="1"/>
       <c r="K234" s="1"/>
@@ -10471,7 +10471,7 @@
       </c>
       <c r="I235" s="1">
         <f t="shared" si="18"/>
-        <v>1.625135427952171E-2</v>
+        <v>1.6238159675235224E-2</v>
       </c>
       <c r="J235" s="1"/>
       <c r="K235" s="1"/>
@@ -10507,7 +10507,7 @@
       </c>
       <c r="I236" s="1">
         <f t="shared" si="18"/>
-        <v>0.44333996023856936</v>
+        <v>0.43372556646893012</v>
       </c>
       <c r="J236" s="1"/>
       <c r="K236" s="1"/>
@@ -10543,7 +10543,7 @@
       </c>
       <c r="I237" s="1">
         <f t="shared" si="18"/>
-        <v>1.3248430986302635</v>
+        <v>1.242534908700323</v>
       </c>
       <c r="J237" s="1"/>
       <c r="K237" s="1"/>
@@ -10579,7 +10579,7 @@
       </c>
       <c r="I238" s="1">
         <f t="shared" si="18"/>
-        <v>-0.22649649469710428</v>
+        <v>-0.22909090909090743</v>
       </c>
       <c r="J238" s="1"/>
       <c r="K238" s="1"/>
@@ -10615,7 +10615,7 @@
       </c>
       <c r="I239" s="1">
         <f t="shared" si="18"/>
-        <v>-0.24986180210060704</v>
+        <v>-0.24677877265778456</v>
       </c>
       <c r="J239" s="1"/>
       <c r="K239" s="1"/>
@@ -10651,7 +10651,7 @@
       </c>
       <c r="I240" s="1">
         <f t="shared" si="18"/>
-        <v>-0.14256919522147554</v>
+        <v>-0.14156008981743795</v>
       </c>
       <c r="J240" s="1"/>
       <c r="K240" s="1"/>
@@ -10687,7 +10687,7 @@
       </c>
       <c r="I241" s="1">
         <f t="shared" si="18"/>
-        <v>0.29183543994924688</v>
+        <v>0.28763828763828847</v>
       </c>
       <c r="J241" s="1"/>
       <c r="K241" s="1"/>
@@ -10723,7 +10723,7 @@
       </c>
       <c r="I242" s="1">
         <f t="shared" si="18"/>
-        <v>2.4521072796934343E-2</v>
+        <v>2.4551173852999323E-2</v>
       </c>
       <c r="J242" s="1"/>
       <c r="K242" s="1"/>
@@ -10759,7 +10759,7 @@
       </c>
       <c r="I243" s="1">
         <f t="shared" si="18"/>
-        <v>0.32229185317815523</v>
+        <v>0.32757051865332065</v>
       </c>
       <c r="J243" s="1"/>
       <c r="K243" s="1"/>
@@ -10795,7 +10795,7 @@
       </c>
       <c r="I244" s="1">
         <f t="shared" si="18"/>
-        <v>7.4471254095918982E-2</v>
+        <v>7.4749588877261172E-2</v>
       </c>
       <c r="J244" s="1"/>
       <c r="K244" s="1"/>
@@ -10831,7 +10831,7 @@
       </c>
       <c r="I245" s="1">
         <f t="shared" si="18"/>
-        <v>0.23316817254444683</v>
+        <v>0.23048112935753304</v>
       </c>
       <c r="J245" s="1"/>
       <c r="K245" s="1"/>
@@ -10867,7 +10867,7 @@
       </c>
       <c r="I246" s="1">
         <f t="shared" si="18"/>
-        <v>0.16443987667009191</v>
+        <v>0.16309887869520839</v>
       </c>
       <c r="J246" s="1"/>
       <c r="K246" s="1"/>
@@ -10903,7 +10903,7 @@
       </c>
       <c r="I247" s="1">
         <f t="shared" si="18"/>
-        <v>-0.11382658185470247</v>
+        <v>-0.11318242343541821</v>
       </c>
       <c r="J247" s="1"/>
       <c r="K247" s="1"/>
@@ -10939,7 +10939,7 @@
       </c>
       <c r="I248" s="1">
         <f t="shared" si="18"/>
-        <v>-1.5681828916914642</v>
+        <v>-1.4541631991590376</v>
       </c>
       <c r="J248" s="1"/>
       <c r="K248" s="1"/>
@@ -10975,7 +10975,7 @@
       </c>
       <c r="I249" s="1">
         <f t="shared" si="18"/>
-        <v>-8.9620675281368661E-2</v>
+        <v>-8.9220873534600453E-2</v>
       </c>
       <c r="J249" s="1"/>
       <c r="K249" s="1"/>
@@ -11011,7 +11011,7 @@
       </c>
       <c r="I250" s="1">
         <f t="shared" si="18"/>
-        <v>-6.7479061644107038E-2</v>
+        <v>-6.7707503584514439E-2</v>
       </c>
       <c r="J250" s="1"/>
       <c r="K250" s="1"/>
@@ -11047,7 +11047,7 @@
       </c>
       <c r="I251" s="1">
         <f t="shared" si="18"/>
-        <v>3.7919509000997914E-2</v>
+        <v>3.7847750595030129E-2</v>
       </c>
       <c r="J251" s="1"/>
       <c r="K251" s="1"/>
@@ -11083,7 +11083,7 @@
       </c>
       <c r="I252" s="1">
         <f t="shared" si="18"/>
-        <v>0.10538099282019679</v>
+        <v>0.10482864548334524</v>
       </c>
       <c r="J252" s="1"/>
       <c r="K252" s="1"/>
@@ -11119,7 +11119,7 @@
       </c>
       <c r="I253" s="1">
         <f t="shared" si="18"/>
-        <v>-6.3009999412950851E-2</v>
+        <v>-6.2812109862672189E-2</v>
       </c>
       <c r="J253" s="1"/>
       <c r="K253" s="1"/>
@@ -11155,7 +11155,7 @@
       </c>
       <c r="I254" s="1">
         <f t="shared" si="18"/>
-        <v>0.12492901760363365</v>
+        <v>0.12571428571428506</v>
       </c>
       <c r="J254" s="1"/>
       <c r="K254" s="1"/>
@@ -11191,7 +11191,7 @@
       </c>
       <c r="I255" s="1">
         <f t="shared" si="18"/>
-        <v>-5.3611738148983554E-2</v>
+        <v>-5.375583533738796E-2</v>
       </c>
       <c r="J255" s="1"/>
       <c r="K255" s="1"/>
@@ -11227,7 +11227,7 @@
       </c>
       <c r="I256" s="1">
         <f t="shared" si="18"/>
-        <v>-4.7762551884916807E-2</v>
+        <v>-4.7876888002281667E-2</v>
       </c>
       <c r="J256" s="1"/>
       <c r="K256" s="1"/>
@@ -11263,7 +11263,7 @@
       </c>
       <c r="I257" s="1">
         <f t="shared" si="18"/>
-        <v>-0.33903726211418594</v>
+        <v>-0.34488368309744666</v>
       </c>
       <c r="J257" s="1"/>
       <c r="K257" s="1"/>
@@ -11299,7 +11299,7 @@
       </c>
       <c r="I258" s="1">
         <f t="shared" si="18"/>
-        <v>-0.10276422764227539</v>
+        <v>-0.10329497907949686</v>
       </c>
       <c r="J258" s="1"/>
       <c r="K258" s="1"/>
@@ -11334,8 +11334,8 @@
         <v>0.21999999999999886</v>
       </c>
       <c r="I259" s="1">
-        <f t="shared" ref="I259:I322" si="23">($L$2/COUNT($B$2:$B$501)) * (H259 / B259)</f>
-        <v>2.3830155979202648E-2</v>
+        <f t="shared" ref="I259:I322" si="23">($L$2/COUNT($B$2:$B$501)) * (H259 / A259)</f>
+        <v>2.3858583667714876E-2</v>
       </c>
       <c r="J259" s="1"/>
       <c r="K259" s="1"/>
@@ -11371,7 +11371,7 @@
       </c>
       <c r="I260" s="1">
         <f t="shared" si="23"/>
-        <v>0.27008860372746812</v>
+        <v>0.26648981068371008</v>
       </c>
       <c r="J260" s="1"/>
       <c r="K260" s="1"/>
@@ -11407,7 +11407,7 @@
       </c>
       <c r="I261" s="1">
         <f t="shared" si="23"/>
-        <v>5.1072522982661475E-3</v>
+        <v>5.10594842992347E-3</v>
       </c>
       <c r="J261" s="1"/>
       <c r="K261" s="1"/>
@@ -11443,7 +11443,7 @@
       </c>
       <c r="I262" s="1">
         <f t="shared" si="23"/>
-        <v>-0.13956796159658577</v>
+        <v>-0.14054876684123302</v>
       </c>
       <c r="J262" s="1"/>
       <c r="K262" s="1"/>
@@ -11479,7 +11479,7 @@
       </c>
       <c r="I263" s="1">
         <f t="shared" si="23"/>
-        <v>-1.727755152412869E-2</v>
+        <v>-1.7292490118578904E-2</v>
       </c>
       <c r="J263" s="1"/>
       <c r="K263" s="1"/>
@@ -11515,7 +11515,7 @@
       </c>
       <c r="I264" s="1">
         <f t="shared" si="23"/>
-        <v>-1.019473081328752</v>
+        <v>-0.97002724795640383</v>
       </c>
       <c r="J264" s="1"/>
       <c r="K264" s="1"/>
@@ -11551,7 +11551,7 @@
       </c>
       <c r="I265" s="1">
         <f t="shared" si="23"/>
-        <v>-0.16260162601626083</v>
+        <v>-0.16393442622950888</v>
       </c>
       <c r="J265" s="1"/>
       <c r="K265" s="1"/>
@@ -11587,7 +11587,7 @@
       </c>
       <c r="I266" s="1">
         <f t="shared" si="23"/>
-        <v>4.6841454687400121E-2</v>
+        <v>4.6951418324096994E-2</v>
       </c>
       <c r="J266" s="1"/>
       <c r="K266" s="1"/>
@@ -11623,7 +11623,7 @@
       </c>
       <c r="I267" s="1">
         <f t="shared" si="23"/>
-        <v>0.27412906910336771</v>
+        <v>0.27042253521126586</v>
       </c>
       <c r="J267" s="1"/>
       <c r="K267" s="1"/>
@@ -11659,7 +11659,7 @@
       </c>
       <c r="I268" s="1">
         <f t="shared" si="23"/>
-        <v>1.6708437761068985E-2</v>
+        <v>1.6694490818029692E-2</v>
       </c>
       <c r="J268" s="1"/>
       <c r="K268" s="1"/>
@@ -11695,7 +11695,7 @@
       </c>
       <c r="I269" s="1">
         <f t="shared" si="23"/>
-        <v>-0.65349437966906077</v>
+        <v>-0.67556838686394494</v>
       </c>
       <c r="J269" s="1"/>
       <c r="K269" s="1"/>
@@ -11731,7 +11731,7 @@
       </c>
       <c r="I270" s="1">
         <f t="shared" si="23"/>
-        <v>4.5635367409742E-2</v>
+        <v>4.5739734890088674E-2</v>
       </c>
       <c r="J270" s="1"/>
       <c r="K270" s="1"/>
@@ -11767,7 +11767,7 @@
       </c>
       <c r="I271" s="1">
         <f t="shared" si="23"/>
-        <v>1.3140604467806018E-2</v>
+        <v>1.3149243918475186E-2</v>
       </c>
       <c r="J271" s="1"/>
       <c r="K271" s="1"/>
@@ -11803,7 +11803,7 @@
       </c>
       <c r="I272" s="1">
         <f t="shared" si="23"/>
-        <v>-0.17607042817126761</v>
+        <v>-0.17763423496164624</v>
       </c>
       <c r="J272" s="1"/>
       <c r="K272" s="1"/>
@@ -11839,7 +11839,7 @@
       </c>
       <c r="I273" s="1">
         <f t="shared" si="23"/>
-        <v>0.1543550165380381</v>
+        <v>0.1555555555555562</v>
       </c>
       <c r="J273" s="1"/>
       <c r="K273" s="1"/>
@@ -11875,7 +11875,7 @@
       </c>
       <c r="I274" s="1">
         <f t="shared" si="23"/>
-        <v>-0.21399910833704824</v>
+        <v>-0.21173356859285367</v>
       </c>
       <c r="J274" s="1"/>
       <c r="K274" s="1"/>
@@ -11911,7 +11911,7 @@
       </c>
       <c r="I275" s="1">
         <f t="shared" si="23"/>
-        <v>0.32989326982446687</v>
+        <v>0.32454009024644059</v>
       </c>
       <c r="J275" s="1"/>
       <c r="K275" s="1"/>
@@ -11947,7 +11947,7 @@
       </c>
       <c r="I276" s="1">
         <f t="shared" si="23"/>
-        <v>-0.16557734204792829</v>
+        <v>-0.16695957820737936</v>
       </c>
       <c r="J276" s="1"/>
       <c r="K276" s="1"/>
@@ -11983,7 +11983,7 @@
       </c>
       <c r="I277" s="1">
         <f t="shared" si="23"/>
-        <v>-3.6380453214122511E-2</v>
+        <v>-3.6446750679517657E-2</v>
       </c>
       <c r="J277" s="1"/>
       <c r="K277" s="1"/>
@@ -12019,7 +12019,7 @@
       </c>
       <c r="I278" s="1">
         <f t="shared" si="23"/>
-        <v>-5.4512057830184021E-2</v>
+        <v>-5.4661042124651893E-2</v>
       </c>
       <c r="J278" s="1"/>
       <c r="K278" s="1"/>
@@ -12055,7 +12055,7 @@
       </c>
       <c r="I279" s="1">
         <f t="shared" si="23"/>
-        <v>0.37192902638762626</v>
+        <v>0.37897664715767637</v>
       </c>
       <c r="J279" s="1"/>
       <c r="K279" s="1"/>
@@ -12091,7 +12091,7 @@
       </c>
       <c r="I280" s="1">
         <f t="shared" si="23"/>
-        <v>-0.88989310854262449</v>
+        <v>-0.93133242382901149</v>
       </c>
       <c r="J280" s="1"/>
       <c r="K280" s="1"/>
@@ -12127,7 +12127,7 @@
       </c>
       <c r="I281" s="1">
         <f t="shared" si="23"/>
-        <v>0.12526096033402931</v>
+        <v>0.12448132780082997</v>
       </c>
       <c r="J281" s="1"/>
       <c r="K281" s="1"/>
@@ -12163,7 +12163,7 @@
       </c>
       <c r="I282" s="1">
         <f t="shared" si="23"/>
-        <v>0.12519495847911424</v>
+        <v>0.12441614477515142</v>
       </c>
       <c r="J282" s="1"/>
       <c r="K282" s="1"/>
@@ -12199,7 +12199,7 @@
       </c>
       <c r="I283" s="1">
         <f t="shared" si="23"/>
-        <v>-5.9094155094282501E-2</v>
+        <v>-5.8920063525674936E-2</v>
       </c>
       <c r="J283" s="1"/>
       <c r="K283" s="1"/>
@@ -12235,7 +12235,7 @@
       </c>
       <c r="I284" s="1">
         <f t="shared" si="23"/>
-        <v>0.26269152253404304</v>
+        <v>0.25928591198450124</v>
       </c>
       <c r="J284" s="1"/>
       <c r="K284" s="1"/>
@@ -12271,7 +12271,7 @@
       </c>
       <c r="I285" s="1">
         <f t="shared" si="23"/>
-        <v>-0.23813742513909164</v>
+        <v>-0.23533531780774039</v>
       </c>
       <c r="J285" s="1"/>
       <c r="K285" s="1"/>
@@ -12307,7 +12307,7 @@
       </c>
       <c r="I286" s="1">
         <f t="shared" si="23"/>
-        <v>3.2304958811194043E-3</v>
+        <v>3.2299741602083709E-3</v>
       </c>
       <c r="J286" s="1"/>
       <c r="K286" s="1"/>
@@ -12343,7 +12343,7 @@
       </c>
       <c r="I287" s="1">
         <f t="shared" si="23"/>
-        <v>9.2862143936322417E-2</v>
+        <v>9.3295324127206758E-2</v>
       </c>
       <c r="J287" s="1"/>
       <c r="K287" s="1"/>
@@ -12379,7 +12379,7 @@
       </c>
       <c r="I288" s="1">
         <f t="shared" si="23"/>
-        <v>0.96904792999869249</v>
+        <v>1.0183914356299737</v>
       </c>
       <c r="J288" s="1"/>
       <c r="K288" s="1"/>
@@ -12415,7 +12415,7 @@
       </c>
       <c r="I289" s="1">
         <f t="shared" si="23"/>
-        <v>-0.39426822947146911</v>
+        <v>-0.4021969025039257</v>
       </c>
       <c r="J289" s="1"/>
       <c r="K289" s="1"/>
@@ -12451,7 +12451,7 @@
       </c>
       <c r="I290" s="1">
         <f t="shared" si="23"/>
-        <v>1.1784975878704349</v>
+        <v>1.1129189716889039</v>
       </c>
       <c r="J290" s="1"/>
       <c r="K290" s="1"/>
@@ -12487,7 +12487,7 @@
       </c>
       <c r="I291" s="1">
         <f t="shared" si="23"/>
-        <v>0.54507337526205446</v>
+        <v>0.56034482758620674</v>
       </c>
       <c r="J291" s="1"/>
       <c r="K291" s="1"/>
@@ -12523,7 +12523,7 @@
       </c>
       <c r="I292" s="1">
         <f t="shared" si="23"/>
-        <v>-6.7174783619685041E-2</v>
+        <v>-6.7401166558649611E-2</v>
       </c>
       <c r="J292" s="1"/>
       <c r="K292" s="1"/>
@@ -12559,7 +12559,7 @@
       </c>
       <c r="I293" s="1">
         <f t="shared" si="23"/>
-        <v>-9.0426133152482352E-2</v>
+        <v>-9.0019129064927567E-2</v>
       </c>
       <c r="J293" s="1"/>
       <c r="K293" s="1"/>
@@ -12595,7 +12595,7 @@
       </c>
       <c r="I294" s="1">
         <f t="shared" si="23"/>
-        <v>-0.29878938782519016</v>
+        <v>-0.30332084023359102</v>
       </c>
       <c r="J294" s="1"/>
       <c r="K294" s="1"/>
@@ -12631,7 +12631,7 @@
       </c>
       <c r="I295" s="1">
         <f t="shared" si="23"/>
-        <v>0.12890839275918894</v>
+        <v>0.1280828450742616</v>
       </c>
       <c r="J295" s="1"/>
       <c r="K295" s="1"/>
@@ -12667,7 +12667,7 @@
       </c>
       <c r="I296" s="1">
         <f t="shared" si="23"/>
-        <v>2.9466401896097592E-2</v>
+        <v>2.94230523218613E-2</v>
       </c>
       <c r="J296" s="1"/>
       <c r="K296" s="1"/>
@@ -12703,7 +12703,7 @@
       </c>
       <c r="I297" s="1">
         <f t="shared" si="23"/>
-        <v>-0.2118351370020716</v>
+        <v>-0.21410286246218224</v>
       </c>
       <c r="J297" s="1"/>
       <c r="K297" s="1"/>
@@ -12739,7 +12739,7 @@
       </c>
       <c r="I298" s="1">
         <f t="shared" si="23"/>
-        <v>0.22442084942084767</v>
+        <v>0.22696766320927211</v>
       </c>
       <c r="J298" s="1"/>
       <c r="K298" s="1"/>
@@ -12775,7 +12775,7 @@
       </c>
       <c r="I299" s="1">
         <f t="shared" si="23"/>
-        <v>0.1996153591086936</v>
+        <v>0.20162775898449214</v>
       </c>
       <c r="J299" s="1"/>
       <c r="K299" s="1"/>
@@ -12811,7 +12811,7 @@
       </c>
       <c r="I300" s="1">
         <f t="shared" si="23"/>
-        <v>0.15424164524421805</v>
+        <v>0.15544041450777416</v>
       </c>
       <c r="J300" s="1"/>
       <c r="K300" s="1"/>
@@ -12847,7 +12847,7 @@
       </c>
       <c r="I301" s="1">
         <f t="shared" si="23"/>
-        <v>-0.12674271229404266</v>
+        <v>-0.12755102040816282</v>
       </c>
       <c r="J301" s="1"/>
       <c r="K301" s="1"/>
@@ -12883,7 +12883,7 @@
       </c>
       <c r="I302" s="1">
         <f t="shared" si="23"/>
-        <v>-8.8260497000856988E-2</v>
+        <v>-8.7872712536791464E-2</v>
       </c>
       <c r="J302" s="1"/>
       <c r="K302" s="1"/>
@@ -12919,7 +12919,7 @@
       </c>
       <c r="I303" s="1">
         <f t="shared" si="23"/>
-        <v>-0.17729482413497416</v>
+        <v>-0.17573696145124845</v>
       </c>
       <c r="J303" s="1"/>
       <c r="K303" s="1"/>
@@ -12955,7 +12955,7 @@
       </c>
       <c r="I304" s="1">
         <f t="shared" si="23"/>
-        <v>0.28134959885701755</v>
+        <v>0.27744662403814913</v>
       </c>
       <c r="J304" s="1"/>
       <c r="K304" s="1"/>
@@ -12991,7 +12991,7 @@
       </c>
       <c r="I305" s="1">
         <f t="shared" si="23"/>
-        <v>-5.4528212422950209E-2</v>
+        <v>-5.4677285153929389E-2</v>
       </c>
       <c r="J305" s="1"/>
       <c r="K305" s="1"/>
@@ -13027,7 +13027,7 @@
       </c>
       <c r="I306" s="1">
         <f t="shared" si="23"/>
-        <v>0.14406988622353439</v>
+        <v>0.14511522290620441</v>
       </c>
       <c r="J306" s="1"/>
       <c r="K306" s="1"/>
@@ -13063,7 +13063,7 @@
       </c>
       <c r="I307" s="1">
         <f t="shared" si="23"/>
-        <v>0.22449488650536434</v>
+        <v>0.22704339051463313</v>
       </c>
       <c r="J307" s="1"/>
       <c r="K307" s="1"/>
@@ -13099,7 +13099,7 @@
       </c>
       <c r="I308" s="1">
         <f t="shared" si="23"/>
-        <v>2.2387568315008349E-2</v>
+        <v>2.2412656559000124E-2</v>
       </c>
       <c r="J308" s="1"/>
       <c r="K308" s="1"/>
@@ -13135,7 +13135,7 @@
       </c>
       <c r="I309" s="1">
         <f t="shared" si="23"/>
-        <v>-0.15234226228259706</v>
+        <v>-0.1511906261811789</v>
       </c>
       <c r="J309" s="1"/>
       <c r="K309" s="1"/>
@@ -13171,7 +13171,7 @@
       </c>
       <c r="I310" s="1">
         <f t="shared" si="23"/>
-        <v>-9.0282563749138692E-2</v>
+        <v>-9.0691958877081397E-2</v>
       </c>
       <c r="J310" s="1"/>
       <c r="K310" s="1"/>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="I311" s="1">
         <f t="shared" si="23"/>
-        <v>-0.26544638473946452</v>
+        <v>-0.26901686241759987</v>
       </c>
       <c r="J311" s="1"/>
       <c r="K311" s="1"/>
@@ -13243,7 +13243,7 @@
       </c>
       <c r="I312" s="1">
         <f t="shared" si="23"/>
-        <v>9.6214369211403805E-2</v>
+        <v>9.5753724998883308E-2</v>
       </c>
       <c r="J312" s="1"/>
       <c r="K312" s="1"/>
@@ -13279,7 +13279,7 @@
       </c>
       <c r="I313" s="1">
         <f t="shared" si="23"/>
-        <v>-0.2277219894046015</v>
+        <v>-0.22515831443984016</v>
       </c>
       <c r="J313" s="1"/>
       <c r="K313" s="1"/>
@@ -13315,7 +13315,7 @@
       </c>
       <c r="I314" s="1">
         <f t="shared" si="23"/>
-        <v>4.491017964072027E-2</v>
+        <v>4.4809559372667868E-2</v>
       </c>
       <c r="J314" s="1"/>
       <c r="K314" s="1"/>
@@ -13351,7 +13351,7 @@
       </c>
       <c r="I315" s="1">
         <f t="shared" si="23"/>
-        <v>5.007511266900351E-2</v>
+        <v>5.0200803212851405E-2</v>
       </c>
       <c r="J315" s="1"/>
       <c r="K315" s="1"/>
@@ -13387,7 +13387,7 @@
       </c>
       <c r="I316" s="1">
         <f t="shared" si="23"/>
-        <v>2.99267138748879</v>
+        <v>3.5192727272727264</v>
       </c>
       <c r="J316" s="1"/>
       <c r="K316" s="1"/>
@@ -13423,7 +13423,7 @@
       </c>
       <c r="I317" s="1">
         <f t="shared" si="23"/>
-        <v>0.19453797231575126</v>
+        <v>0.19644880997355615</v>
       </c>
       <c r="J317" s="1"/>
       <c r="K317" s="1"/>
@@ -13459,7 +13459,7 @@
       </c>
       <c r="I318" s="1">
         <f t="shared" si="23"/>
-        <v>-0.11380731244685782</v>
+        <v>-0.11316337148803389</v>
       </c>
       <c r="J318" s="1"/>
       <c r="K318" s="1"/>
@@ -13495,7 +13495,7 @@
       </c>
       <c r="I319" s="1">
         <f t="shared" si="23"/>
-        <v>0.36421008188615905</v>
+        <v>0.37096555158209193</v>
       </c>
       <c r="J319" s="1"/>
       <c r="K319" s="1"/>
@@ -13531,7 +13531,7 @@
       </c>
       <c r="I320" s="1">
         <f t="shared" si="23"/>
-        <v>-9.2548871470392841E-2</v>
+        <v>-9.2122579432223142E-2</v>
       </c>
       <c r="J320" s="1"/>
       <c r="K320" s="1"/>
@@ -13567,7 +13567,7 @@
       </c>
       <c r="I321" s="1">
         <f t="shared" si="23"/>
-        <v>-0.22348484848484979</v>
+        <v>-0.22101517138040958</v>
       </c>
       <c r="J321" s="1"/>
       <c r="K321" s="1"/>
@@ -13603,7 +13603,7 @@
       </c>
       <c r="I322" s="1">
         <f t="shared" si="23"/>
-        <v>-3.7878787878788414E-2</v>
+        <v>-3.7807183364839861E-2</v>
       </c>
       <c r="J322" s="1"/>
       <c r="K322" s="1"/>
@@ -13638,8 +13638,8 @@
         <v>-0.89499999999999602</v>
       </c>
       <c r="I323" s="1">
-        <f t="shared" ref="I323:I386" si="28">($L$2/COUNT($B$2:$B$501)) * (H323 / B323)</f>
-        <v>-0.15019928676316274</v>
+        <f t="shared" ref="I323:I386" si="28">($L$2/COUNT($B$2:$B$501)) * (H323 / A323)</f>
+        <v>-0.15133581332431451</v>
       </c>
       <c r="J323" s="1"/>
       <c r="K323" s="1"/>
@@ -13675,7 +13675,7 @@
       </c>
       <c r="I324" s="1">
         <f t="shared" si="28"/>
-        <v>0.20907812473526233</v>
+        <v>0.20691505416009787</v>
       </c>
       <c r="J324" s="1"/>
       <c r="K324" s="1"/>
@@ -13711,7 +13711,7 @@
       </c>
       <c r="I325" s="1">
         <f t="shared" si="28"/>
-        <v>-3.7675426203251424E-3</v>
+        <v>-3.7682524729149357E-3</v>
       </c>
       <c r="J325" s="1"/>
       <c r="K325" s="1"/>
@@ -13747,7 +13747,7 @@
       </c>
       <c r="I326" s="1">
         <f t="shared" si="28"/>
-        <v>6.9177390594451063E-2</v>
+        <v>6.8938939796178683E-2</v>
       </c>
       <c r="J326" s="1"/>
       <c r="K326" s="1"/>
@@ -13783,7 +13783,7 @@
       </c>
       <c r="I327" s="1">
         <f t="shared" si="28"/>
-        <v>-6.1712522499356583E-2</v>
+        <v>-6.1903533660045841E-2</v>
       </c>
       <c r="J327" s="1"/>
       <c r="K327" s="1"/>
@@ -13819,7 +13819,7 @@
       </c>
       <c r="I328" s="1">
         <f t="shared" si="28"/>
-        <v>-0.10692328254477565</v>
+        <v>-0.10635469290082576</v>
       </c>
       <c r="J328" s="1"/>
       <c r="K328" s="1"/>
@@ -13855,7 +13855,7 @@
       </c>
       <c r="I329" s="1">
         <f t="shared" si="28"/>
-        <v>-0.45769710491861648</v>
+        <v>-0.44745711364410901</v>
       </c>
       <c r="J329" s="1"/>
       <c r="K329" s="1"/>
@@ -13891,7 +13891,7 @@
       </c>
       <c r="I330" s="1">
         <f t="shared" si="28"/>
-        <v>-0.33508049419693109</v>
+        <v>-0.34079009995240483</v>
       </c>
       <c r="J330" s="1"/>
       <c r="K330" s="1"/>
@@ -13927,7 +13927,7 @@
       </c>
       <c r="I331" s="1">
         <f t="shared" si="28"/>
-        <v>0.16372253339077786</v>
+        <v>0.16239316239316046</v>
       </c>
       <c r="J331" s="1"/>
       <c r="K331" s="1"/>
@@ -13963,7 +13963,7 @@
       </c>
       <c r="I332" s="1">
         <f t="shared" si="28"/>
-        <v>-0.35092383357703238</v>
+        <v>-0.35719117846029158</v>
       </c>
       <c r="J332" s="1"/>
       <c r="K332" s="1"/>
@@ -13999,7 +13999,7 @@
       </c>
       <c r="I333" s="1">
         <f t="shared" si="28"/>
-        <v>-8.1137532133675361E-2</v>
+        <v>-8.0809697163658906E-2</v>
       </c>
       <c r="J333" s="1"/>
       <c r="K333" s="1"/>
@@ -14035,7 +14035,7 @@
       </c>
       <c r="I334" s="1">
         <f t="shared" si="28"/>
-        <v>-0.51678338565563897</v>
+        <v>-0.50376647834274968</v>
       </c>
       <c r="J334" s="1"/>
       <c r="K334" s="1"/>
@@ -14071,7 +14071,7 @@
       </c>
       <c r="I335" s="1">
         <f t="shared" si="28"/>
-        <v>3.4524300316205707</v>
+        <v>2.9441981295462427</v>
       </c>
       <c r="J335" s="1"/>
       <c r="K335" s="1"/>
@@ -14107,7 +14107,7 @@
       </c>
       <c r="I336" s="1">
         <f t="shared" si="28"/>
-        <v>-0.139157632464813</v>
+        <v>-0.14013265891710819</v>
       </c>
       <c r="J336" s="1"/>
       <c r="K336" s="1"/>
@@ -14143,7 +14143,7 @@
       </c>
       <c r="I337" s="1">
         <f t="shared" si="28"/>
-        <v>3.4042553191490653E-2</v>
+        <v>3.3984706881904428E-2</v>
       </c>
       <c r="J337" s="1"/>
       <c r="K337" s="1"/>
@@ -14179,7 +14179,7 @@
       </c>
       <c r="I338" s="1">
         <f t="shared" si="28"/>
-        <v>-0.2453211937278702</v>
+        <v>-0.2423485321673951</v>
       </c>
       <c r="J338" s="1"/>
       <c r="K338" s="1"/>
@@ -14215,7 +14215,7 @@
       </c>
       <c r="I339" s="1">
         <f t="shared" si="28"/>
-        <v>0.29158079535913239</v>
+        <v>0.29589465530596387</v>
       </c>
       <c r="J339" s="1"/>
       <c r="K339" s="1"/>
@@ -14251,7 +14251,7 @@
       </c>
       <c r="I340" s="1">
         <f t="shared" si="28"/>
-        <v>-1.0263592466397715</v>
+        <v>-1.0818790763264592</v>
       </c>
       <c r="J340" s="1"/>
       <c r="K340" s="1"/>
@@ -14287,7 +14287,7 @@
       </c>
       <c r="I341" s="1">
         <f t="shared" si="28"/>
-        <v>0.34942322768507161</v>
+        <v>0.3556366123332958</v>
       </c>
       <c r="J341" s="1"/>
       <c r="K341" s="1"/>
@@ -14323,7 +14323,7 @@
       </c>
       <c r="I342" s="1">
         <f t="shared" si="28"/>
-        <v>0.28175683674677571</v>
+        <v>0.27784263366799139</v>
       </c>
       <c r="J342" s="1"/>
       <c r="K342" s="1"/>
@@ -14359,7 +14359,7 @@
       </c>
       <c r="I343" s="1">
         <f t="shared" si="28"/>
-        <v>0.13851802403204244</v>
+        <v>0.13948407696832169</v>
       </c>
       <c r="J343" s="1"/>
       <c r="K343" s="1"/>
@@ -14395,7 +14395,7 @@
       </c>
       <c r="I344" s="1">
         <f t="shared" si="28"/>
-        <v>-5.4480007782858469E-2</v>
+        <v>-5.46288167008099E-2</v>
       </c>
       <c r="J344" s="1"/>
       <c r="K344" s="1"/>
@@ -14431,7 +14431,7 @@
       </c>
       <c r="I345" s="1">
         <f t="shared" si="28"/>
-        <v>-4.3862752033958584E-2</v>
+        <v>-4.3766765494847142E-2</v>
       </c>
       <c r="J345" s="1"/>
       <c r="K345" s="1"/>
@@ -14467,7 +14467,7 @@
       </c>
       <c r="I346" s="1">
         <f t="shared" si="28"/>
-        <v>-0.11965811965812014</v>
+        <v>-0.12037833190025843</v>
       </c>
       <c r="J346" s="1"/>
       <c r="K346" s="1"/>
@@ -14503,7 +14503,7 @@
       </c>
       <c r="I347" s="1">
         <f t="shared" si="28"/>
-        <v>9.8228814984072391E-2</v>
+        <v>9.8713641183885203E-2</v>
       </c>
       <c r="J347" s="1"/>
       <c r="K347" s="1"/>
@@ -14539,7 +14539,7 @@
       </c>
       <c r="I348" s="1">
         <f t="shared" si="28"/>
-        <v>-4.330566582461369E-2</v>
+        <v>-4.3399638336348849E-2</v>
       </c>
       <c r="J348" s="1"/>
       <c r="K348" s="1"/>
@@ -14575,7 +14575,7 @@
       </c>
       <c r="I349" s="1">
         <f t="shared" si="28"/>
-        <v>6.1633281972266446E-2</v>
+        <v>6.1823802163834506E-2</v>
       </c>
       <c r="J349" s="1"/>
       <c r="K349" s="1"/>
@@ -14611,7 +14611,7 @@
       </c>
       <c r="I350" s="1">
         <f t="shared" si="28"/>
-        <v>-0.23005814196678798</v>
+        <v>-0.23273527420446855</v>
       </c>
       <c r="J350" s="1"/>
       <c r="K350" s="1"/>
@@ -14647,7 +14647,7 @@
       </c>
       <c r="I351" s="1">
         <f t="shared" si="28"/>
-        <v>0.29379244984994235</v>
+        <v>0.28953922789538999</v>
       </c>
       <c r="J351" s="1"/>
       <c r="K351" s="1"/>
@@ -14683,7 +14683,7 @@
       </c>
       <c r="I352" s="1">
         <f t="shared" si="28"/>
-        <v>0.32740733017048274</v>
+        <v>0.33285630995918963</v>
       </c>
       <c r="J352" s="1"/>
       <c r="K352" s="1"/>
@@ -14719,7 +14719,7 @@
       </c>
       <c r="I353" s="1">
         <f t="shared" si="28"/>
-        <v>-0.14161108260646438</v>
+        <v>-0.14262091773460059</v>
       </c>
       <c r="J353" s="1"/>
       <c r="K353" s="1"/>
@@ -14755,7 +14755,7 @@
       </c>
       <c r="I354" s="1">
         <f t="shared" si="28"/>
-        <v>-5.3758088601293386E-2</v>
+        <v>-5.3613979348688653E-2</v>
       </c>
       <c r="J354" s="1"/>
       <c r="K354" s="1"/>
@@ -14791,7 +14791,7 @@
       </c>
       <c r="I355" s="1">
         <f t="shared" si="28"/>
-        <v>0.60493651020117123</v>
+        <v>0.62380461968515655</v>
       </c>
       <c r="J355" s="1"/>
       <c r="K355" s="1"/>
@@ -14827,7 +14827,7 @@
       </c>
       <c r="I356" s="1">
         <f t="shared" si="28"/>
-        <v>-0.13997246443322614</v>
+        <v>-0.1409589832466781</v>
       </c>
       <c r="J356" s="1"/>
       <c r="K356" s="1"/>
@@ -14863,7 +14863,7 @@
       </c>
       <c r="I357" s="1">
         <f t="shared" si="28"/>
-        <v>-8.6683280962181388E-3</v>
+        <v>-8.6720867208669051E-3</v>
       </c>
       <c r="J357" s="1"/>
       <c r="K357" s="1"/>
@@ -14899,7 +14899,7 @@
       </c>
       <c r="I358" s="1">
         <f t="shared" si="28"/>
-        <v>-7.4160811865729009E-2</v>
+        <v>-7.3886836476763654E-2</v>
       </c>
       <c r="J358" s="1"/>
       <c r="K358" s="1"/>
@@ -14935,7 +14935,7 @@
       </c>
       <c r="I359" s="1">
         <f t="shared" si="28"/>
-        <v>1.168451801363238E-2</v>
+        <v>1.1691348402182828E-2</v>
       </c>
       <c r="J359" s="1"/>
       <c r="K359" s="1"/>
@@ -14971,7 +14971,7 @@
       </c>
       <c r="I360" s="1">
         <f t="shared" si="28"/>
-        <v>-0.3440706799100029</v>
+        <v>-0.35009352578240499</v>
       </c>
       <c r="J360" s="1"/>
       <c r="K360" s="1"/>
@@ -15007,7 +15007,7 @@
       </c>
       <c r="I361" s="1">
         <f t="shared" si="28"/>
-        <v>-3.8872691933919047E-2</v>
+        <v>-3.8797284190109305E-2</v>
       </c>
       <c r="J361" s="1"/>
       <c r="K361" s="1"/>
@@ -15043,7 +15043,7 @@
       </c>
       <c r="I362" s="1">
         <f t="shared" si="28"/>
-        <v>9.3242915960282183E-2</v>
+        <v>9.3679664213152908E-2</v>
       </c>
       <c r="J362" s="1"/>
       <c r="K362" s="1"/>
@@ -15079,7 +15079,7 @@
       </c>
       <c r="I363" s="1">
         <f t="shared" si="28"/>
-        <v>-3.5290796160361376E-2</v>
+        <v>-3.5353178250724739E-2</v>
       </c>
       <c r="J363" s="1"/>
       <c r="K363" s="1"/>
@@ -15115,7 +15115,7 @@
       </c>
       <c r="I364" s="1">
         <f t="shared" si="28"/>
-        <v>-0.19650863302489768</v>
+        <v>-0.19845857418111776</v>
       </c>
       <c r="J364" s="1"/>
       <c r="K364" s="1"/>
@@ -15151,7 +15151,7 @@
       </c>
       <c r="I365" s="1">
         <f t="shared" si="28"/>
-        <v>-0.10633156114065054</v>
+        <v>-0.10689990281827308</v>
       </c>
       <c r="J365" s="1"/>
       <c r="K365" s="1"/>
@@ -15187,7 +15187,7 @@
       </c>
       <c r="I366" s="1">
         <f t="shared" si="28"/>
-        <v>-5.7477616889577782E-2</v>
+        <v>-5.7312906425659671E-2</v>
       </c>
       <c r="J366" s="1"/>
       <c r="K366" s="1"/>
@@ -15223,7 +15223,7 @@
       </c>
       <c r="I367" s="1">
         <f t="shared" si="28"/>
-        <v>9.1775092936802055E-2</v>
+        <v>9.1355883203237009E-2</v>
       </c>
       <c r="J367" s="1"/>
       <c r="K367" s="1"/>
@@ -15259,7 +15259,7 @@
       </c>
       <c r="I368" s="1">
         <f t="shared" si="28"/>
-        <v>0.15011345784604635</v>
+        <v>0.1489951489951489</v>
       </c>
       <c r="J368" s="1"/>
       <c r="K368" s="1"/>
@@ -15295,7 +15295,7 @@
       </c>
       <c r="I369" s="1">
         <f t="shared" si="28"/>
-        <v>-1.5616285554937508E-2</v>
+        <v>-1.5628488501899393E-2</v>
       </c>
       <c r="J369" s="1"/>
       <c r="K369" s="1"/>
@@ -15331,7 +15331,7 @@
       </c>
       <c r="I370" s="1">
         <f t="shared" si="28"/>
-        <v>8.2522841143522763E-3</v>
+        <v>8.2556905295427738E-3</v>
       </c>
       <c r="J370" s="1"/>
       <c r="K370" s="1"/>
@@ -15367,7 +15367,7 @@
       </c>
       <c r="I371" s="1">
         <f t="shared" si="28"/>
-        <v>-3.2408345148876298E-2</v>
+        <v>-3.2355915065723412E-2</v>
       </c>
       <c r="J371" s="1"/>
       <c r="K371" s="1"/>
@@ -15403,7 +15403,7 @@
       </c>
       <c r="I372" s="1">
         <f t="shared" si="28"/>
-        <v>-0.17913508836583397</v>
+        <v>-0.17754486263300084</v>
       </c>
       <c r="J372" s="1"/>
       <c r="K372" s="1"/>
@@ -15439,7 +15439,7 @@
       </c>
       <c r="I373" s="1">
         <f t="shared" si="28"/>
-        <v>0.39746798174591735</v>
+        <v>0.40552718534094584</v>
       </c>
       <c r="J373" s="1"/>
       <c r="K373" s="1"/>
@@ -15475,7 +15475,7 @@
       </c>
       <c r="I374" s="1">
         <f t="shared" si="28"/>
-        <v>0.10816990590097776</v>
+        <v>0.10758801661928871</v>
       </c>
       <c r="J374" s="1"/>
       <c r="K374" s="1"/>
@@ -15511,7 +15511,7 @@
       </c>
       <c r="I375" s="1">
         <f t="shared" si="28"/>
-        <v>-7.4763249709254506E-2</v>
+        <v>-7.4484813374162517E-2</v>
       </c>
       <c r="J375" s="1"/>
       <c r="K375" s="1"/>
@@ -15547,7 +15547,7 @@
       </c>
       <c r="I376" s="1">
         <f t="shared" si="28"/>
-        <v>-0.44311789691194869</v>
+        <v>-0.45315801831415647</v>
       </c>
       <c r="J376" s="1"/>
       <c r="K376" s="1"/>
@@ -15583,7 +15583,7 @@
       </c>
       <c r="I377" s="1">
         <f t="shared" si="28"/>
-        <v>-0.20933734939759255</v>
+        <v>-0.21155163229587015</v>
       </c>
       <c r="J377" s="1"/>
       <c r="K377" s="1"/>
@@ -15619,7 +15619,7 @@
       </c>
       <c r="I378" s="1">
         <f t="shared" si="28"/>
-        <v>-7.4109364247524082E-2</v>
+        <v>-7.4384995483766911E-2</v>
       </c>
       <c r="J378" s="1"/>
       <c r="K378" s="1"/>
@@ -15655,7 +15655,7 @@
       </c>
       <c r="I379" s="1">
         <f t="shared" si="28"/>
-        <v>-0.27772187562889827</v>
+        <v>-0.28163265306122354</v>
       </c>
       <c r="J379" s="1"/>
       <c r="K379" s="1"/>
@@ -15691,7 +15691,7 @@
       </c>
       <c r="I380" s="1">
         <f t="shared" si="28"/>
-        <v>6.9180986386967708E-2</v>
+        <v>6.9421117456052464E-2</v>
       </c>
       <c r="J380" s="1"/>
       <c r="K380" s="1"/>
@@ -15727,7 +15727,7 @@
       </c>
       <c r="I381" s="1">
         <f t="shared" si="28"/>
-        <v>-0.24313296596979656</v>
+        <v>-0.24612502129109065</v>
       </c>
       <c r="J381" s="1"/>
       <c r="K381" s="1"/>
@@ -15763,7 +15763,7 @@
       </c>
       <c r="I382" s="1">
         <f t="shared" si="28"/>
-        <v>1.4130492394127296</v>
+        <v>1.5204745066727483</v>
       </c>
       <c r="J382" s="1"/>
       <c r="K382" s="1"/>
@@ -15799,7 +15799,7 @@
       </c>
       <c r="I383" s="1">
         <f t="shared" si="28"/>
-        <v>0.14777550699575503</v>
+        <v>0.1488755147291729</v>
       </c>
       <c r="J383" s="1"/>
       <c r="K383" s="1"/>
@@ -15835,7 +15835,7 @@
       </c>
       <c r="I384" s="1">
         <f t="shared" si="28"/>
-        <v>0.15206812652068125</v>
+        <v>0.15092061575611226</v>
       </c>
       <c r="J384" s="1"/>
       <c r="K384" s="1"/>
@@ -15871,7 +15871,7 @@
       </c>
       <c r="I385" s="1">
         <f t="shared" si="28"/>
-        <v>-2.8721876495932157E-2</v>
+        <v>-2.8763183125600323E-2</v>
       </c>
       <c r="J385" s="1"/>
       <c r="K385" s="1"/>
@@ -15907,7 +15907,7 @@
       </c>
       <c r="I386" s="1">
         <f t="shared" si="28"/>
-        <v>-7.9189197175189852E-2</v>
+        <v>-7.8876887306117388E-2</v>
       </c>
       <c r="J386" s="1"/>
       <c r="K386" s="1"/>
@@ -15942,8 +15942,8 @@
         <v>-0.62000000000000455</v>
       </c>
       <c r="I387" s="1">
-        <f t="shared" ref="I387:I450" si="33">($L$2/COUNT($B$2:$B$501)) * (H387 / B387)</f>
-        <v>-9.6498054474708883E-2</v>
+        <f t="shared" ref="I387:I450" si="33">($L$2/COUNT($B$2:$B$501)) * (H387 / A387)</f>
+        <v>-9.6034696406444311E-2</v>
       </c>
       <c r="J387" s="1"/>
       <c r="K387" s="1"/>
@@ -15979,7 +15979,7 @@
       </c>
       <c r="I388" s="1">
         <f t="shared" si="33"/>
-        <v>-7.6227812261780653E-3</v>
+        <v>-7.6256876736198248E-3</v>
       </c>
       <c r="J388" s="1"/>
       <c r="K388" s="1"/>
@@ -16015,7 +16015,7 @@
       </c>
       <c r="I389" s="1">
         <f t="shared" si="33"/>
-        <v>-0.21997161656560602</v>
+        <v>-0.22241789779212898</v>
       </c>
       <c r="J389" s="1"/>
       <c r="K389" s="1"/>
@@ -16051,7 +16051,7 @@
       </c>
       <c r="I390" s="1">
         <f t="shared" si="33"/>
-        <v>-0.13760904287996123</v>
+        <v>-0.13856241494494675</v>
       </c>
       <c r="J390" s="1"/>
       <c r="K390" s="1"/>
@@ -16087,7 +16087,7 @@
       </c>
       <c r="I391" s="1">
         <f t="shared" si="33"/>
-        <v>0.18200202224469175</v>
+        <v>0.18367346938775525</v>
       </c>
       <c r="J391" s="1"/>
       <c r="K391" s="1"/>
@@ -16123,7 +16123,7 @@
       </c>
       <c r="I392" s="1">
         <f t="shared" si="33"/>
-        <v>-0.13457868835994813</v>
+        <v>-0.13367916999201951</v>
       </c>
       <c r="J392" s="1"/>
       <c r="K392" s="1"/>
@@ -16159,7 +16159,7 @@
       </c>
       <c r="I393" s="1">
         <f t="shared" si="33"/>
-        <v>-0.17836905641783712</v>
+        <v>-0.17997414736004796</v>
       </c>
       <c r="J393" s="1"/>
       <c r="K393" s="1"/>
@@ -16195,7 +16195,7 @@
       </c>
       <c r="I394" s="1">
         <f t="shared" si="33"/>
-        <v>6.3888888888889994E-2</v>
+        <v>6.3685449259311633E-2</v>
       </c>
       <c r="J394" s="1"/>
       <c r="K394" s="1"/>
@@ -16231,7 +16231,7 @@
       </c>
       <c r="I395" s="1">
         <f t="shared" si="33"/>
-        <v>-0.25106510676881799</v>
+        <v>-0.2479524957775191</v>
       </c>
       <c r="J395" s="1"/>
       <c r="K395" s="1"/>
@@ -16267,7 +16267,7 @@
       </c>
       <c r="I396" s="1">
         <f t="shared" si="33"/>
-        <v>-9.179333866688974E-2</v>
+        <v>-9.2216582064296282E-2</v>
       </c>
       <c r="J396" s="1"/>
       <c r="K396" s="1"/>
@@ -16303,7 +16303,7 @@
       </c>
       <c r="I397" s="1">
         <f t="shared" si="33"/>
-        <v>-1.3546898330392276</v>
+        <v>-1.4531158998252749</v>
       </c>
       <c r="J397" s="1"/>
       <c r="K397" s="1"/>
@@ -16339,7 +16339,7 @@
       </c>
       <c r="I398" s="1">
         <f t="shared" si="33"/>
-        <v>-0.13646012331952115</v>
+        <v>-0.13739758790901457</v>
       </c>
       <c r="J398" s="1"/>
       <c r="K398" s="1"/>
@@ -16375,7 +16375,7 @@
       </c>
       <c r="I399" s="1">
         <f t="shared" si="33"/>
-        <v>0.15050167224080124</v>
+        <v>0.15164279696714261</v>
       </c>
       <c r="J399" s="1"/>
       <c r="K399" s="1"/>
@@ -16411,7 +16411,7 @@
       </c>
       <c r="I400" s="1">
         <f t="shared" si="33"/>
-        <v>8.5952389850142197E-2</v>
+        <v>8.6323374868636643E-2</v>
       </c>
       <c r="J400" s="1"/>
       <c r="K400" s="1"/>
@@ -16447,7 +16447,7 @@
       </c>
       <c r="I401" s="1">
         <f t="shared" si="33"/>
-        <v>-1.4162720619888072</v>
+        <v>-1.3226130653266326</v>
       </c>
       <c r="J401" s="1"/>
       <c r="K401" s="1"/>
@@ -16483,7 +16483,7 @@
       </c>
       <c r="I402" s="1">
         <f t="shared" si="33"/>
-        <v>-3.0251604810744851E-2</v>
+        <v>-3.0205915939147971E-2</v>
       </c>
       <c r="J402" s="1"/>
       <c r="K402" s="1"/>
@@ -16519,7 +16519,7 @@
       </c>
       <c r="I403" s="1">
         <f t="shared" si="33"/>
-        <v>-0.11913007341737272</v>
+        <v>-0.11842467639768846</v>
       </c>
       <c r="J403" s="1"/>
       <c r="K403" s="1"/>
@@ -16555,7 +16555,7 @@
       </c>
       <c r="I404" s="1">
         <f t="shared" si="33"/>
-        <v>0.25218427323272358</v>
+        <v>0.24904402392391334</v>
       </c>
       <c r="J404" s="1"/>
       <c r="K404" s="1"/>
@@ -16591,7 +16591,7 @@
       </c>
       <c r="I405" s="1">
         <f t="shared" si="33"/>
-        <v>0.32595669888950901</v>
+        <v>0.320729502397609</v>
       </c>
       <c r="J405" s="1"/>
       <c r="K405" s="1"/>
@@ -16627,7 +16627,7 @@
       </c>
       <c r="I406" s="1">
         <f t="shared" si="33"/>
-        <v>-0.40640606164973292</v>
+        <v>-0.3983122362869197</v>
       </c>
       <c r="J406" s="1"/>
       <c r="K406" s="1"/>
@@ -16663,7 +16663,7 @@
       </c>
       <c r="I407" s="1">
         <f t="shared" si="33"/>
-        <v>-0.19344089080342958</v>
+        <v>-0.19533013254544673</v>
       </c>
       <c r="J407" s="1"/>
       <c r="K407" s="1"/>
@@ -16699,7 +16699,7 @@
       </c>
       <c r="I408" s="1">
         <f t="shared" si="33"/>
-        <v>0.10293360782295419</v>
+        <v>0.10240655401945725</v>
       </c>
       <c r="J408" s="1"/>
       <c r="K408" s="1"/>
@@ -16735,7 +16735,7 @@
       </c>
       <c r="I409" s="1">
         <f t="shared" si="33"/>
-        <v>-0.24245763879322485</v>
+        <v>-0.24543299400362845</v>
       </c>
       <c r="J409" s="1"/>
       <c r="K409" s="1"/>
@@ -16771,7 +16771,7 @@
       </c>
       <c r="I410" s="1">
         <f t="shared" si="33"/>
-        <v>-6.1946902654867506E-2</v>
+        <v>-6.1755624172915996E-2</v>
       </c>
       <c r="J410" s="1"/>
       <c r="K410" s="1"/>
@@ -16807,7 +16807,7 @@
       </c>
       <c r="I411" s="1">
         <f t="shared" si="33"/>
-        <v>-0.11278195488721746</v>
+        <v>-0.11214953271027979</v>
       </c>
       <c r="J411" s="1"/>
       <c r="K411" s="1"/>
@@ -16843,7 +16843,7 @@
       </c>
       <c r="I412" s="1">
         <f t="shared" si="33"/>
-        <v>-0.43092620522096914</v>
+        <v>-0.42183717066223769</v>
       </c>
       <c r="J412" s="1"/>
       <c r="K412" s="1"/>
@@ -16879,7 +16879,7 @@
       </c>
       <c r="I413" s="1">
         <f t="shared" si="33"/>
-        <v>-0.37255792821444672</v>
+        <v>-0.37962962962962837</v>
       </c>
       <c r="J413" s="1"/>
       <c r="K413" s="1"/>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="I414" s="1">
         <f t="shared" si="33"/>
-        <v>-3.2231823553787377E-2</v>
+        <v>-3.2283851924731106E-2</v>
       </c>
       <c r="J414" s="1"/>
       <c r="K414" s="1"/>
@@ -16951,7 +16951,7 @@
       </c>
       <c r="I415" s="1">
         <f t="shared" si="33"/>
-        <v>7.4305906108025233E-2</v>
+        <v>7.4583003992621744E-2</v>
       </c>
       <c r="J415" s="1"/>
       <c r="K415" s="1"/>
@@ -16987,7 +16987,7 @@
       </c>
       <c r="I416" s="1">
         <f t="shared" si="33"/>
-        <v>0.11322367015594982</v>
+        <v>0.11258629845990464</v>
       </c>
       <c r="J416" s="1"/>
       <c r="K416" s="1"/>
@@ -17023,7 +17023,7 @@
       </c>
       <c r="I417" s="1">
         <f t="shared" si="33"/>
-        <v>-0.20342685507543298</v>
+        <v>-0.2055172413793116</v>
       </c>
       <c r="J417" s="1"/>
       <c r="K417" s="1"/>
@@ -17059,7 +17059,7 @@
       </c>
       <c r="I418" s="1">
         <f t="shared" si="33"/>
-        <v>5.3068758652512628E-2</v>
+        <v>5.2928316649405074E-2</v>
       </c>
       <c r="J418" s="1"/>
       <c r="K418" s="1"/>
@@ -17095,7 +17095,7 @@
       </c>
       <c r="I419" s="1">
         <f t="shared" si="33"/>
-        <v>-0.72403512685825633</v>
+        <v>-0.69873952869333844</v>
       </c>
       <c r="J419" s="1"/>
       <c r="K419" s="1"/>
@@ -17131,7 +17131,7 @@
       </c>
       <c r="I420" s="1">
         <f t="shared" si="33"/>
-        <v>4.4304535385332335E-2</v>
+        <v>4.4206607724522506E-2</v>
       </c>
       <c r="J420" s="1"/>
       <c r="K420" s="1"/>
@@ -17167,7 +17167,7 @@
       </c>
       <c r="I421" s="1">
         <f t="shared" si="33"/>
-        <v>0.54113506379234533</v>
+        <v>0.55618358580149274</v>
       </c>
       <c r="J421" s="1"/>
       <c r="K421" s="1"/>
@@ -17203,7 +17203,7 @@
       </c>
       <c r="I422" s="1">
         <f t="shared" si="33"/>
-        <v>0.26539848124568816</v>
+        <v>0.26896766169154518</v>
       </c>
       <c r="J422" s="1"/>
       <c r="K422" s="1"/>
@@ -17239,7 +17239,7 @@
       </c>
       <c r="I423" s="1">
         <f t="shared" si="33"/>
-        <v>-9.3620727193553799E-2</v>
+        <v>-9.4061030296399992E-2</v>
       </c>
       <c r="J423" s="1"/>
       <c r="K423" s="1"/>
@@ -17275,7 +17275,7 @@
       </c>
       <c r="I424" s="1">
         <f t="shared" si="33"/>
-        <v>8.6563431759161841E-2</v>
+        <v>8.6939721792890806E-2</v>
       </c>
       <c r="J424" s="1"/>
       <c r="K424" s="1"/>
@@ -17311,7 +17311,7 @@
       </c>
       <c r="I425" s="1">
         <f t="shared" si="33"/>
-        <v>-6.3159644311476013E-2</v>
+        <v>-6.2960815176869425E-2</v>
       </c>
       <c r="J425" s="1"/>
       <c r="K425" s="1"/>
@@ -17347,7 +17347,7 @@
       </c>
       <c r="I426" s="1">
         <f t="shared" si="33"/>
-        <v>-0.34009156311314637</v>
+        <v>-0.33440514469453425</v>
       </c>
       <c r="J426" s="1"/>
       <c r="K426" s="1"/>
@@ -17383,7 +17383,7 @@
       </c>
       <c r="I427" s="1">
         <f t="shared" si="33"/>
-        <v>-7.77529400330461E-2</v>
+        <v>-7.7451834640334144E-2</v>
       </c>
       <c r="J427" s="1"/>
       <c r="K427" s="1"/>
@@ -17419,7 +17419,7 @@
       </c>
       <c r="I428" s="1">
         <f t="shared" si="33"/>
-        <v>3.3648790746581829E-2</v>
+        <v>3.3705498209394689E-2</v>
       </c>
       <c r="J428" s="1"/>
       <c r="K428" s="1"/>
@@ -17455,7 +17455,7 @@
       </c>
       <c r="I429" s="1">
         <f t="shared" si="33"/>
-        <v>-9.4100615273252988E-2</v>
+        <v>-9.4545454545453822E-2</v>
       </c>
       <c r="J429" s="1"/>
       <c r="K429" s="1"/>
@@ -17491,7 +17491,7 @@
       </c>
       <c r="I430" s="1">
         <f t="shared" si="33"/>
-        <v>0.18336389398233099</v>
+        <v>0.18169805087545485</v>
       </c>
       <c r="J430" s="1"/>
       <c r="K430" s="1"/>
@@ -17527,7 +17527,7 @@
       </c>
       <c r="I431" s="1">
         <f t="shared" si="33"/>
-        <v>-6.9920666935589862E-2</v>
+        <v>-6.9677073562907921E-2</v>
       </c>
       <c r="J431" s="1"/>
       <c r="K431" s="1"/>
@@ -17563,7 +17563,7 @@
       </c>
       <c r="I432" s="1">
         <f t="shared" si="33"/>
-        <v>0.27496055893621796</v>
+        <v>0.27123165851489528</v>
       </c>
       <c r="J432" s="1"/>
       <c r="K432" s="1"/>
@@ -17599,7 +17599,7 @@
       </c>
       <c r="I433" s="1">
         <f t="shared" si="33"/>
-        <v>-2.1390374331551613E-2</v>
+        <v>-2.1413276231264197E-2</v>
       </c>
       <c r="J433" s="1"/>
       <c r="K433" s="1"/>
@@ -17635,7 +17635,7 @@
       </c>
       <c r="I434" s="1">
         <f t="shared" si="33"/>
-        <v>-0.17881030946223095</v>
+        <v>-0.17722581928269909</v>
       </c>
       <c r="J434" s="1"/>
       <c r="K434" s="1"/>
@@ -17671,7 +17671,7 @@
       </c>
       <c r="I435" s="1">
         <f t="shared" si="33"/>
-        <v>-0.12682576253989727</v>
+        <v>-0.12763513369780255</v>
       </c>
       <c r="J435" s="1"/>
       <c r="K435" s="1"/>
@@ -17707,7 +17707,7 @@
       </c>
       <c r="I436" s="1">
         <f t="shared" si="33"/>
-        <v>-0.28968544257498441</v>
+        <v>-0.28554946639746437</v>
       </c>
       <c r="J436" s="1"/>
       <c r="K436" s="1"/>
@@ -17743,7 +17743,7 @@
       </c>
       <c r="I437" s="1">
         <f t="shared" si="33"/>
-        <v>0.19199346405228712</v>
+        <v>0.19385440296968401</v>
       </c>
       <c r="J437" s="1"/>
       <c r="K437" s="1"/>
@@ -17779,7 +17779,7 @@
       </c>
       <c r="I438" s="1">
         <f t="shared" si="33"/>
-        <v>-2.470428893905193</v>
+        <v>-2.1988266495218207</v>
       </c>
       <c r="J438" s="1"/>
       <c r="K438" s="1"/>
@@ -17815,7 +17815,7 @@
       </c>
       <c r="I439" s="1">
         <f t="shared" si="33"/>
-        <v>1.3821700069109025E-2</v>
+        <v>1.381215469613312E-2</v>
       </c>
       <c r="J439" s="1"/>
       <c r="K439" s="1"/>
@@ -17851,7 +17851,7 @@
       </c>
       <c r="I440" s="1">
         <f t="shared" si="33"/>
-        <v>-0.18845500848896427</v>
+        <v>-0.1866958203683457</v>
       </c>
       <c r="J440" s="1"/>
       <c r="K440" s="1"/>
@@ -17887,7 +17887,7 @@
       </c>
       <c r="I441" s="1">
         <f t="shared" si="33"/>
-        <v>0.28497236833344253</v>
+        <v>0.28909152313407449</v>
       </c>
       <c r="J441" s="1"/>
       <c r="K441" s="1"/>
@@ -17923,7 +17923,7 @@
       </c>
       <c r="I442" s="1">
         <f t="shared" si="33"/>
-        <v>-5.254400560469592E-3</v>
+        <v>-5.2530204867800969E-3</v>
       </c>
       <c r="J442" s="1"/>
       <c r="K442" s="1"/>
@@ -17959,7 +17959,7 @@
       </c>
       <c r="I443" s="1">
         <f t="shared" si="33"/>
-        <v>-0.68385268105412556</v>
+        <v>-0.66124303977519328</v>
       </c>
       <c r="J443" s="1"/>
       <c r="K443" s="1"/>
@@ -17995,7 +17995,7 @@
       </c>
       <c r="I444" s="1">
         <f t="shared" si="33"/>
-        <v>-1.0798081863332774</v>
+        <v>-1.1414347137361407</v>
       </c>
       <c r="J444" s="1"/>
       <c r="K444" s="1"/>
@@ -18031,7 +18031,7 @@
       </c>
       <c r="I445" s="1">
         <f t="shared" si="33"/>
-        <v>0.42266187050359616</v>
+        <v>0.43178686265502886</v>
       </c>
       <c r="J445" s="1"/>
       <c r="K445" s="1"/>
@@ -18067,7 +18067,7 @@
       </c>
       <c r="I446" s="1">
         <f t="shared" si="33"/>
-        <v>-0.32506821687032972</v>
+        <v>-0.33043897732754568</v>
       </c>
       <c r="J446" s="1"/>
       <c r="K446" s="1"/>
@@ -18103,7 +18103,7 @@
       </c>
       <c r="I447" s="1">
         <f t="shared" si="33"/>
-        <v>8.5865257595774472E-2</v>
+        <v>8.6235489220565537E-2</v>
       </c>
       <c r="J447" s="1"/>
       <c r="K447" s="1"/>
@@ -18139,7 +18139,7 @@
       </c>
       <c r="I448" s="1">
         <f t="shared" si="33"/>
-        <v>-0.44107142857142839</v>
+        <v>-0.45101798593992493</v>
       </c>
       <c r="J448" s="1"/>
       <c r="K448" s="1"/>
@@ -18175,7 +18175,7 @@
       </c>
       <c r="I449" s="1">
         <f t="shared" si="33"/>
-        <v>7.1754474905433518E-2</v>
+        <v>7.1497959976686676E-2</v>
       </c>
       <c r="J449" s="1"/>
       <c r="K449" s="1"/>
@@ -18211,7 +18211,7 @@
       </c>
       <c r="I450" s="1">
         <f t="shared" si="33"/>
-        <v>-1.2831535995336605</v>
+        <v>-1.2057927351158861</v>
       </c>
       <c r="J450" s="1"/>
       <c r="K450" s="1"/>
@@ -18246,8 +18246,8 @@
         <v>46.890000000000015</v>
       </c>
       <c r="I451" s="1">
-        <f t="shared" ref="I451:I501" si="38">($L$2/COUNT($B$2:$B$501)) * (H451 / B451)</f>
-        <v>3.5994473017578881</v>
+        <f t="shared" ref="I451:I501" si="38">($L$2/COUNT($B$2:$B$501)) * (H451 / A451)</f>
+        <v>4.3894219517903128</v>
       </c>
       <c r="J451" s="1"/>
       <c r="K451" s="1"/>
@@ -18283,7 +18283,7 @@
       </c>
       <c r="I452" s="1">
         <f t="shared" si="38"/>
-        <v>-5.0821616127392368E-2</v>
+        <v>-5.0951086956521258E-2</v>
       </c>
       <c r="J452" s="1"/>
       <c r="K452" s="1"/>
@@ -18319,7 +18319,7 @@
       </c>
       <c r="I453" s="1">
         <f t="shared" si="38"/>
-        <v>0.16659873649887824</v>
+        <v>0.16522244397847469</v>
       </c>
       <c r="J453" s="1"/>
       <c r="K453" s="1"/>
@@ -18355,7 +18355,7 @@
       </c>
       <c r="I454" s="1">
         <f t="shared" si="38"/>
-        <v>-3.4720069440139022E-2</v>
+        <v>-3.4780448419352981E-2</v>
       </c>
       <c r="J454" s="1"/>
       <c r="K454" s="1"/>
@@ -18391,7 +18391,7 @@
       </c>
       <c r="I455" s="1">
         <f t="shared" si="38"/>
-        <v>0.47236472751911679</v>
+        <v>0.48379101814216274</v>
       </c>
       <c r="J455" s="1"/>
       <c r="K455" s="1"/>
@@ -18427,7 +18427,7 @@
       </c>
       <c r="I456" s="1">
         <f t="shared" si="38"/>
-        <v>-1.3125613346418077</v>
+        <v>-1.2317255669391063</v>
       </c>
       <c r="J456" s="1"/>
       <c r="K456" s="1"/>
@@ -18463,7 +18463,7 @@
       </c>
       <c r="I457" s="1">
         <f t="shared" si="38"/>
-        <v>0.96822698744769886</v>
+        <v>1.0174847995603038</v>
       </c>
       <c r="J457" s="1"/>
       <c r="K457" s="1"/>
@@ -18499,7 +18499,7 @@
       </c>
       <c r="I458" s="1">
         <f t="shared" si="38"/>
-        <v>-0.27923211169284257</v>
+        <v>-0.28318584070796243</v>
       </c>
       <c r="J458" s="1"/>
       <c r="K458" s="1"/>
@@ -18535,7 +18535,7 @@
       </c>
       <c r="I459" s="1">
         <f t="shared" si="38"/>
-        <v>0.36609477645258048</v>
+        <v>0.35951396718025863</v>
       </c>
       <c r="J459" s="1"/>
       <c r="K459" s="1"/>
@@ -18571,7 +18571,7 @@
       </c>
       <c r="I460" s="1">
         <f t="shared" si="38"/>
-        <v>8.5354896675650369E-2</v>
+        <v>8.4992171773651412E-2</v>
       </c>
       <c r="J460" s="1"/>
       <c r="K460" s="1"/>
@@ -18607,7 +18607,7 @@
       </c>
       <c r="I461" s="1">
         <f t="shared" si="38"/>
-        <v>0.83181353142653747</v>
+        <v>0.79859924837717755</v>
       </c>
       <c r="J461" s="1"/>
       <c r="K461" s="1"/>
@@ -18643,7 +18643,7 @@
       </c>
       <c r="I462" s="1">
         <f t="shared" si="38"/>
-        <v>1.4702278853224353E-2</v>
+        <v>1.4713094654244382E-2</v>
       </c>
       <c r="J462" s="1"/>
       <c r="K462" s="1"/>
@@ -18679,7 +18679,7 @@
       </c>
       <c r="I463" s="1">
         <f t="shared" si="38"/>
-        <v>-0.13299816369827666</v>
+        <v>-0.13211958061773937</v>
       </c>
       <c r="J463" s="1"/>
       <c r="K463" s="1"/>
@@ -18715,7 +18715,7 @@
       </c>
       <c r="I464" s="1">
         <f t="shared" si="38"/>
-        <v>-0.9196498223108247</v>
+        <v>-0.8792210482701458</v>
       </c>
       <c r="J464" s="1"/>
       <c r="K464" s="1"/>
@@ -18751,7 +18751,7 @@
       </c>
       <c r="I465" s="1">
         <f t="shared" si="38"/>
-        <v>1.0018794274974709</v>
+        <v>1.0547142531009828</v>
       </c>
       <c r="J465" s="1"/>
       <c r="K465" s="1"/>
@@ -18787,7 +18787,7 @@
       </c>
       <c r="I466" s="1">
         <f t="shared" si="38"/>
-        <v>0.22499696932961505</v>
+        <v>0.22249394615071025</v>
       </c>
       <c r="J466" s="1"/>
       <c r="K466" s="1"/>
@@ -18823,7 +18823,7 @@
       </c>
       <c r="I467" s="1">
         <f t="shared" si="38"/>
-        <v>3.3023735810112809E-2</v>
+        <v>3.2969297341849696E-2</v>
       </c>
       <c r="J467" s="1"/>
       <c r="K467" s="1"/>
@@ -18859,7 +18859,7 @@
       </c>
       <c r="I468" s="1">
         <f t="shared" si="38"/>
-        <v>3.45959685106089E-2</v>
+        <v>3.4536227798139918E-2</v>
       </c>
       <c r="J468" s="1"/>
       <c r="K468" s="1"/>
@@ -18895,7 +18895,7 @@
       </c>
       <c r="I469" s="1">
         <f t="shared" si="38"/>
-        <v>2.1338210638624414E-2</v>
+        <v>2.1315468940318934E-2</v>
       </c>
       <c r="J469" s="1"/>
       <c r="K469" s="1"/>
@@ -18931,7 +18931,7 @@
       </c>
       <c r="I470" s="1">
         <f t="shared" si="38"/>
-        <v>-0.22601879684943271</v>
+        <v>-0.22349311460606297</v>
       </c>
       <c r="J470" s="1"/>
       <c r="K470" s="1"/>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="I471" s="1">
         <f t="shared" si="38"/>
-        <v>-0.96975425330813037</v>
+        <v>-0.92490759938700251</v>
       </c>
       <c r="J471" s="1"/>
       <c r="K471" s="1"/>
@@ -19003,7 +19003,7 @@
       </c>
       <c r="I472" s="1">
         <f t="shared" si="38"/>
-        <v>-0.19835227050876733</v>
+        <v>-0.20033915684032183</v>
       </c>
       <c r="J472" s="1"/>
       <c r="K472" s="1"/>
@@ -19039,7 +19039,7 @@
       </c>
       <c r="I473" s="1">
         <f t="shared" si="38"/>
-        <v>-0.12379694281939886</v>
+        <v>-0.1230353726696415</v>
       </c>
       <c r="J473" s="1"/>
       <c r="K473" s="1"/>
@@ -19075,7 +19075,7 @@
       </c>
       <c r="I474" s="1">
         <f t="shared" si="38"/>
-        <v>-7.1316656761575087E-2</v>
+        <v>-7.1063257065948487E-2</v>
       </c>
       <c r="J474" s="1"/>
       <c r="K474" s="1"/>
@@ -19111,7 +19111,7 @@
       </c>
       <c r="I475" s="1">
         <f t="shared" si="38"/>
-        <v>-7.9250720461095298E-2</v>
+        <v>-7.9566003616636724E-2</v>
       </c>
       <c r="J475" s="1"/>
       <c r="K475" s="1"/>
@@ -19147,7 +19147,7 @@
       </c>
       <c r="I476" s="1">
         <f t="shared" si="38"/>
-        <v>-8.7607518317935201E-2</v>
+        <v>-8.7225438109586412E-2</v>
       </c>
       <c r="J476" s="1"/>
       <c r="K476" s="1"/>
@@ -19183,7 +19183,7 @@
       </c>
       <c r="I477" s="1">
         <f t="shared" si="38"/>
-        <v>-3.0321406913279055E-2</v>
+        <v>-3.0367446097781452E-2</v>
       </c>
       <c r="J477" s="1"/>
       <c r="K477" s="1"/>
@@ -19219,7 +19219,7 @@
       </c>
       <c r="I478" s="1">
         <f t="shared" si="38"/>
-        <v>0.104438642297651</v>
+        <v>0.10389610389610475</v>
       </c>
       <c r="J478" s="1"/>
       <c r="K478" s="1"/>
@@ -19255,7 +19255,7 @@
       </c>
       <c r="I479" s="1">
         <f t="shared" si="38"/>
-        <v>-0.47778308647873863</v>
+        <v>-0.46663555762949138</v>
       </c>
       <c r="J479" s="1"/>
       <c r="K479" s="1"/>
@@ -19291,7 +19291,7 @@
       </c>
       <c r="I480" s="1">
         <f t="shared" si="38"/>
-        <v>-0.18195281921083242</v>
+        <v>-0.18362335859933798</v>
       </c>
       <c r="J480" s="1"/>
       <c r="K480" s="1"/>
@@ -19327,7 +19327,7 @@
       </c>
       <c r="I481" s="1">
         <f t="shared" si="38"/>
-        <v>-0.36541399327833557</v>
+        <v>-0.35885741718674757</v>
       </c>
       <c r="J481" s="1"/>
       <c r="K481" s="1"/>
@@ -19363,7 +19363,7 @@
       </c>
       <c r="I482" s="1">
         <f t="shared" si="38"/>
-        <v>4.287245444801624E-2</v>
+        <v>4.2780748663100693E-2</v>
       </c>
       <c r="J482" s="1"/>
       <c r="K482" s="1"/>
@@ -19399,7 +19399,7 @@
       </c>
       <c r="I483" s="1">
         <f t="shared" si="38"/>
-        <v>0.53120849933598979</v>
+        <v>0.54570259208731287</v>
       </c>
       <c r="J483" s="1"/>
       <c r="K483" s="1"/>
@@ -19435,7 +19435,7 @@
       </c>
       <c r="I484" s="1">
         <f t="shared" si="38"/>
-        <v>-4.5139933794765483E-2</v>
+        <v>-4.5038282540160839E-2</v>
       </c>
       <c r="J484" s="1"/>
       <c r="K484" s="1"/>
@@ -19471,7 +19471,7 @@
       </c>
       <c r="I485" s="1">
         <f t="shared" si="38"/>
-        <v>0.14573423742536157</v>
+        <v>0.144679995981111</v>
       </c>
       <c r="J485" s="1"/>
       <c r="K485" s="1"/>
@@ -19507,7 +19507,7 @@
       </c>
       <c r="I486" s="1">
         <f t="shared" si="38"/>
-        <v>-4.6941247728649639E-2</v>
+        <v>-4.7051680959247513E-2</v>
       </c>
       <c r="J486" s="1"/>
       <c r="K486" s="1"/>
@@ -19543,7 +19543,7 @@
       </c>
       <c r="I487" s="1">
         <f t="shared" si="38"/>
-        <v>-0.25989909799724642</v>
+        <v>-0.26332094175960169</v>
       </c>
       <c r="J487" s="1"/>
       <c r="K487" s="1"/>
@@ -19579,7 +19579,7 @@
       </c>
       <c r="I488" s="1">
         <f t="shared" si="38"/>
-        <v>0.27473316421768096</v>
+        <v>0.27101038715769638</v>
       </c>
       <c r="J488" s="1"/>
       <c r="K488" s="1"/>
@@ -19615,7 +19615,7 @@
       </c>
       <c r="I489" s="1">
         <f t="shared" si="38"/>
-        <v>-0.14251781472684086</v>
+        <v>-0.14354066985645933</v>
       </c>
       <c r="J489" s="1"/>
       <c r="K489" s="1"/>
@@ -19651,7 +19651,7 @@
       </c>
       <c r="I490" s="1">
         <f t="shared" si="38"/>
-        <v>5.0565856007703767E-2</v>
+        <v>5.0438333133179719E-2</v>
       </c>
       <c r="J490" s="1"/>
       <c r="K490" s="1"/>
@@ -19687,7 +19687,7 @@
       </c>
       <c r="I491" s="1">
         <f t="shared" si="38"/>
-        <v>-5.7335581787519262E-2</v>
+        <v>-5.7500422797224615E-2</v>
       </c>
       <c r="J491" s="1"/>
       <c r="K491" s="1"/>
@@ -19723,7 +19723,7 @@
       </c>
       <c r="I492" s="1">
         <f t="shared" si="38"/>
-        <v>2.6625911690827109</v>
+        <v>3.0714983940790397</v>
       </c>
       <c r="J492" s="1"/>
       <c r="K492" s="1"/>
@@ -19759,7 +19759,7 @@
       </c>
       <c r="I493" s="1">
         <f t="shared" si="38"/>
-        <v>-8.6699236221013609E-2</v>
+        <v>-8.6325020553575688E-2</v>
       </c>
       <c r="J493" s="1"/>
       <c r="K493" s="1"/>
@@ -19795,7 +19795,7 @@
       </c>
       <c r="I494" s="1">
         <f t="shared" si="38"/>
-        <v>0.16811955168119308</v>
+        <v>0.1695447409733099</v>
       </c>
       <c r="J494" s="1"/>
       <c r="K494" s="1"/>
@@ -19831,7 +19831,7 @@
       </c>
       <c r="I495" s="1">
         <f t="shared" si="38"/>
-        <v>4.6981922173422487E-2</v>
+        <v>4.7092547092544991E-2</v>
       </c>
       <c r="J495" s="1"/>
       <c r="K495" s="1"/>
@@ -19867,7 +19867,7 @@
       </c>
       <c r="I496" s="1">
         <f t="shared" si="38"/>
-        <v>0.24873330262551893</v>
+        <v>0.25186567164179174</v>
       </c>
       <c r="J496" s="1"/>
       <c r="K496" s="1"/>
@@ -19903,7 +19903,7 @@
       </c>
       <c r="I497" s="1">
         <f t="shared" si="38"/>
-        <v>-0.10699657276602868</v>
+        <v>-0.10642720545439438</v>
       </c>
       <c r="J497" s="1"/>
       <c r="K497" s="1"/>
@@ -19939,7 +19939,7 @@
       </c>
       <c r="I498" s="1">
         <f t="shared" si="38"/>
-        <v>-0.1653398652786302</v>
+        <v>-0.16398420892803106</v>
       </c>
       <c r="J498" s="1"/>
       <c r="K498" s="1"/>
@@ -19975,7 +19975,7 @@
       </c>
       <c r="I499" s="1">
         <f t="shared" si="38"/>
-        <v>-0.11859190872926827</v>
+        <v>-0.11789285181316526</v>
       </c>
       <c r="J499" s="1"/>
       <c r="K499" s="1"/>
@@ -20011,7 +20011,7 @@
       </c>
       <c r="I500" s="1">
         <f t="shared" si="38"/>
-        <v>-0.13461538461538516</v>
+        <v>-0.13371537726838639</v>
       </c>
       <c r="J500" s="1"/>
       <c r="K500" s="1"/>
@@ -20047,7 +20047,7 @@
       </c>
       <c r="I501" s="1">
         <f t="shared" si="38"/>
-        <v>0.3325323832408088</v>
+        <v>0.32709391724849801</v>
       </c>
       <c r="J501" s="1"/>
       <c r="K501" s="1"/>

</xml_diff>